<commit_message>
index with cleaning steps for all vaccines
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="249">
   <si>
     <t>status</t>
   </si>
@@ -935,6 +935,44 @@
   </si>
   <si>
     <t>Table_7_components</t>
+  </si>
+  <si>
+    <t>D3_all_vaccines_curated</t>
+  </si>
+  <si>
+    <t>01_T2_42_clean_all_vaccines</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>conceptsetdataset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>D3_all_clean_vaccines D3_vaccines_curated</t>
+  </si>
+  <si>
+    <t>Flowchart_criteria_for_doses_all_vaccines</t>
+  </si>
+  <si>
+    <t>01_T2_43_curate_all_vaccines</t>
   </si>
 </sst>
 </file>
@@ -1469,13 +1507,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B34" sqref="A34:XFD34"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1672,204 +1710,204 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>38</v>
+        <v>31</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>244</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>41</v>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>248</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="16" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D16" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C20" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D20" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E20" s="9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
+    <row r="21" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B21" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C21" s="20" t="s">
         <v>57</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>63</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="31" t="s">
-        <v>65</v>
+      <c r="B22" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D22" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E22" s="35" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>11</v>
-      </c>
       <c r="E23" s="35" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="31" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="E24" s="35" t="s">
         <v>64</v>
@@ -1877,13 +1915,13 @@
     </row>
     <row r="25" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="31" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="E25" s="35" t="s">
         <v>64</v>
@@ -1891,488 +1929,488 @@
     </row>
     <row r="26" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="31" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="E26" s="35" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="19" t="s">
-        <v>72</v>
+      <c r="B27" s="31" t="s">
+        <v>68</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E27" s="31" t="s">
-        <v>75</v>
+        <v>61</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="19" t="s">
-        <v>76</v>
+      <c r="B28" s="31" t="s">
+        <v>69</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" t="s">
-        <v>81</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E28" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="19" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B32" s="19" t="s">
+    <row r="34" spans="2:8" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B34" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B35" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C35" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D35" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="E35" s="19" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="2:8" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B33" s="36" t="s">
+    <row r="36" spans="2:8" s="19" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B36" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C36" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D36" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E36" s="19" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="2:8" s="25" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B34" s="23" t="s">
+    <row r="37" spans="2:8" s="25" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B37" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C37" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="D34" s="25" t="s">
+      <c r="D37" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="39" t="s">
+      <c r="E37" s="39" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="2:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="37" t="s">
+    <row r="38" spans="2:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C38" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D38" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E35" s="38" t="s">
+      <c r="E38" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="H35" s="19" t="s">
+      <c r="H38" s="19" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="2:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="37" t="s">
+    <row r="39" spans="2:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C39" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D39" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E36" s="38" t="s">
+      <c r="E39" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="H36" s="19" t="s">
+      <c r="H39" s="19" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="2:8" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B37" s="19" t="s">
+    <row r="40" spans="2:8" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B40" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C40" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D40" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E37" s="38" t="s">
+      <c r="E40" s="38" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="D38" t="s">
-        <v>45</v>
-      </c>
-      <c r="E38" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>104</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39" t="s">
-        <v>106</v>
-      </c>
-      <c r="E39" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>107</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="D40" t="s">
-        <v>45</v>
-      </c>
-      <c r="E40" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D41" t="s">
-        <v>106</v>
+        <v>45</v>
       </c>
       <c r="E41" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D42" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="E42" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D43" t="s">
         <v>45</v>
       </c>
       <c r="E43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" t="s">
+        <v>106</v>
+      </c>
+      <c r="E44" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B44" s="21" t="s">
+      <c r="C45" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" t="s">
+        <v>45</v>
+      </c>
+      <c r="E45" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D46" t="s">
+        <v>45</v>
+      </c>
+      <c r="E46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B47" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="C47" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="F44" s="21"/>
-    </row>
-    <row r="45" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B45" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="C45" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="F45" s="21"/>
-    </row>
-    <row r="46" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B46" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="C46" s="22" t="s">
-        <v>229</v>
-      </c>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="F46" s="21"/>
-    </row>
-    <row r="47" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B47" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="C47" s="22" t="s">
-        <v>230</v>
       </c>
       <c r="D47" s="21"/>
       <c r="E47" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="F47" s="21"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B48" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="F48" s="21"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B49" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="F47" s="21"/>
-    </row>
-    <row r="48" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
+      <c r="C49" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="F49" s="21"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B50" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="F50" s="21"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
         <v>116</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C51" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D51" t="s">
         <v>106</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E51" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B49" t="s">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
         <v>118</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C52" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D52" t="s">
         <v>106</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E52" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B50" s="21" t="s">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="C50" s="22" t="s">
+      <c r="C53" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="D50" s="21" t="s">
+      <c r="D53" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="21" t="s">
+      <c r="E53" s="21" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="51" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B51" s="21" t="s">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B54" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="C51" s="22" t="s">
+      <c r="C54" s="22" t="s">
         <v>235</v>
       </c>
-      <c r="D51" s="21" t="s">
+      <c r="D54" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="E51" s="21" t="s">
+      <c r="E54" s="21" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="52" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B52" s="29" t="s">
+    <row r="55" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B55" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C55" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D55" t="s">
         <v>121</v>
       </c>
-      <c r="E52" s="13" t="s">
+      <c r="E55" s="13" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B53" s="29" t="s">
+    <row r="56" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B56" s="29" t="s">
         <v>237</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C56" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D56" t="s">
         <v>121</v>
       </c>
-      <c r="E53" s="13" t="s">
+      <c r="E56" s="13" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B54" s="29" t="s">
+    <row r="57" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B57" s="29" t="s">
         <v>238</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C57" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D57" t="s">
         <v>121</v>
       </c>
-      <c r="E54" s="13" t="s">
+      <c r="E57" s="13" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="55" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B55" s="26" t="s">
+    <row r="58" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B58" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="C55" s="27" t="s">
+      <c r="C58" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D55" s="28" t="s">
+      <c r="D58" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="E55" s="27" t="s">
+      <c r="E58" s="27" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B56" s="30" t="s">
+    <row r="59" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B59" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="C56" s="27" t="s">
+      <c r="C59" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D56" s="28" t="s">
+      <c r="D59" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="E56" s="27" t="s">
+      <c r="E59" s="27" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="57" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B57" s="33" t="s">
+    <row r="60" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B60" s="33" t="s">
         <v>239</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="D57" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="E57" s="22" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" s="25" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B58" s="34" t="s">
-        <v>241</v>
-      </c>
-      <c r="C58" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="D58" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="E58" s="24" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B59" s="33" t="s">
-        <v>240</v>
-      </c>
-      <c r="C59" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="D59" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="E59" s="22" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B60" s="33" t="s">
-        <v>242</v>
       </c>
       <c r="C60" s="22" t="s">
         <v>120</v>
@@ -2381,6 +2419,48 @@
         <v>121</v>
       </c>
       <c r="E60" s="22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" s="25" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B61" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D61" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="E61" s="24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B62" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D62" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E62" s="22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B63" s="33" t="s">
+        <v>242</v>
+      </c>
+      <c r="C63" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E63" s="22" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3378,27 +3458,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -3649,10 +3708,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3669,20 +3760,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added target cohorts (still no codebooks)
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="252">
   <si>
     <t>status</t>
   </si>
@@ -451,27 +451,6 @@
     <t>04_T2_30_create_study_population_cohort</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D3_TD_variable_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>condition</t>
-    </r>
-  </si>
-  <si>
     <t>04_T2_40_create_TD_datasets</t>
   </si>
   <si>
@@ -974,12 +953,48 @@
   <si>
     <t>01_T2_43_curate_all_vaccines</t>
   </si>
+  <si>
+    <t>04_T2_31_create_study_population_target_cohorts</t>
+  </si>
+  <si>
+    <t>D3_study_population_target_cohorts</t>
+  </si>
+  <si>
+    <r>
+      <t>D3_TD_variable_</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>condition</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D3_study_population_cohort D3_TD_variable_</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>condition</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1063,6 +1078,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -1132,7 +1154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1193,6 +1215,8 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1507,13 +1531,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1713,41 +1737,41 @@
         <v>31</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13" s="32" t="s">
         <v>247</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>248</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -2028,7 +2052,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>83</v>
       </c>
@@ -2042,7 +2066,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="2:8" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="19" t="s">
         <v>86</v>
       </c>
@@ -2056,7 +2080,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="2:8" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35" s="19" t="s">
         <v>87</v>
       </c>
@@ -2098,29 +2122,29 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="2:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="37" t="s">
+    <row r="38" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="40" t="s">
+        <v>250</v>
+      </c>
+      <c r="C38" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="D38" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="H38" s="21" t="s">
         <v>94</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E38" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="H38" s="19" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="39" spans="2:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>74</v>
@@ -2129,339 +2153,350 @@
         <v>50</v>
       </c>
       <c r="H39" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="19" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B40" s="19" t="s">
+      <c r="C40" s="20" t="s">
         <v>98</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>99</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>74</v>
       </c>
       <c r="E40" s="38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="C41" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="E41" s="34" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
+      <c r="C42" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="D42" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" t="s">
         <v>102</v>
       </c>
-      <c r="D41" t="s">
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" t="s">
+        <v>105</v>
+      </c>
+      <c r="E43" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" t="s">
         <v>45</v>
       </c>
-      <c r="E41" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>104</v>
-      </c>
-      <c r="C42" s="13" t="s">
+      <c r="E44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" t="s">
         <v>105</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E45" t="s">
         <v>106</v>
-      </c>
-      <c r="E42" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>107</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="D43" t="s">
-        <v>45</v>
-      </c>
-      <c r="E43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>109</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="D44" t="s">
-        <v>106</v>
-      </c>
-      <c r="E44" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>111</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="D45" t="s">
-        <v>45</v>
-      </c>
-      <c r="E45" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D46" t="s">
         <v>45</v>
       </c>
       <c r="E46" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B47" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="C47" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="F47" s="21"/>
+      <c r="B47" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" t="s">
+        <v>45</v>
+      </c>
+      <c r="E47" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B48" s="21" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D48" s="21"/>
       <c r="E48" s="21" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F48" s="21"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="21" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D49" s="21"/>
       <c r="E49" s="21" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="F49" s="21"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="C50" s="22" t="s">
         <v>228</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>230</v>
       </c>
       <c r="D50" s="21"/>
       <c r="E50" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="F50" s="21"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B51" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="F50" s="21"/>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B51" t="s">
-        <v>116</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D51" t="s">
-        <v>106</v>
-      </c>
-      <c r="E51" t="s">
-        <v>114</v>
-      </c>
+      <c r="C51" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="F51" s="21"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
+        <v>115</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D52" t="s">
+        <v>105</v>
+      </c>
+      <c r="E52" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C52" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="D52" t="s">
-        <v>106</v>
-      </c>
-      <c r="E52" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B53" s="21" t="s">
-        <v>232</v>
-      </c>
-      <c r="C53" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="D53" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="E53" s="21" t="s">
-        <v>228</v>
+      <c r="D53" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="C54" s="22" t="s">
         <v>233</v>
       </c>
-      <c r="C54" s="22" t="s">
-        <v>235</v>
-      </c>
       <c r="D54" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B55" s="29" t="s">
-        <v>236</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="D55" t="s">
-        <v>121</v>
-      </c>
-      <c r="E55" s="13" t="s">
-        <v>122</v>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B55" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E55" s="21" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B56" s="29" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C56" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D56" t="s">
         <v>120</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" s="13" t="s">
         <v>121</v>
-      </c>
-      <c r="E56" s="13" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="57" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B57" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D57" t="s">
+        <v>120</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B58" s="29" t="s">
+        <v>237</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D58" t="s">
+        <v>120</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B59" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="D59" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="E59" s="27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B60" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C60" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="D60" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="E60" s="27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B61" s="33" t="s">
         <v>238</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="C61" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D61" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E61" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="E57" s="13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B58" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="C58" s="27" t="s">
+    </row>
+    <row r="62" spans="2:6" s="25" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B62" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="C62" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="D62" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="D58" s="28" t="s">
+      <c r="E62" s="24" t="s">
         <v>121</v>
-      </c>
-      <c r="E58" s="27" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B59" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="C59" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="D59" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="E59" s="27" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B60" s="33" t="s">
-        <v>239</v>
-      </c>
-      <c r="C60" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="D60" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="E60" s="22" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" s="25" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B61" s="34" t="s">
-        <v>241</v>
-      </c>
-      <c r="C61" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="D61" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="E61" s="24" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B62" s="33" t="s">
-        <v>240</v>
-      </c>
-      <c r="C62" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="D62" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="E62" s="22" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="63" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B63" s="33" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C63" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D63" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="D63" s="21" t="s">
+      <c r="E63" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="E63" s="22" t="s">
-        <v>122</v>
+    </row>
+    <row r="64" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B64" s="33" t="s">
+        <v>241</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="E64" s="22" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2475,10 +2510,10 @@
   <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2490,16 +2525,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2507,10 +2542,10 @@
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" t="s">
         <v>129</v>
-      </c>
-      <c r="D2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2518,10 +2553,10 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" t="s">
         <v>131</v>
-      </c>
-      <c r="D3" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2529,7 +2564,7 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2537,7 +2572,7 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2545,911 +2580,911 @@
         <v>82</v>
       </c>
       <c r="C6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" t="s">
         <v>135</v>
-      </c>
-      <c r="D6" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" t="s">
         <v>137</v>
-      </c>
-      <c r="B7" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" t="s">
         <v>139</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>140</v>
       </c>
-      <c r="C8" t="s">
-        <v>141</v>
-      </c>
       <c r="D8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" t="s">
         <v>153</v>
       </c>
-      <c r="C20" t="s">
-        <v>154</v>
-      </c>
       <c r="D20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B27" t="s">
         <v>161</v>
       </c>
-      <c r="B27" t="s">
-        <v>162</v>
-      </c>
       <c r="C27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B36" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B39" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B42" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B43" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B44" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B45" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C45" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B46" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B47" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B48" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B49" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B50" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B51" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B52" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C52" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B53" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C53" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B54" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C54" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B55" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B56" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C56" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B57" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C57" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B58" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B59" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C59" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B60" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C60" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B61" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B62" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C62" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B63" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C63" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B64" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C64" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B65" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C65" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B66" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C66" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B67" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C67" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B68" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C68" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B69" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C69" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B70" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C70" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B71" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C71" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B72" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C72" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B73" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C73" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B74" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C74" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B75" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C75" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B76" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C76" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B77" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C77" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B78" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C78" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B79" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C79" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B80" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C80" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B81" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C81" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B82" t="s">
         <v>218</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>219</v>
-      </c>
-      <c r="C82" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -3709,6 +3744,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
@@ -3718,15 +3762,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3749,6 +3784,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3757,12 +3800,4 @@
     <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
partially updated codebooks on vaccine indicators
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="260">
   <si>
     <t>status</t>
   </si>
@@ -853,16 +853,10 @@
     <t xml:space="preserve">E_DM1_AESI </t>
   </si>
   <si>
-    <t>05_T3_41_count_prevalence_vaccination_dose</t>
-  </si>
-  <si>
     <t>D3_study_population_cohort D3_vaccines_curated</t>
   </si>
   <si>
     <t>D4_count_vaccination_prevalence</t>
-  </si>
-  <si>
-    <t>D4_vaccination_prevalence_aggregated</t>
   </si>
   <si>
     <t>05_T3_42_aggregate_prevalence_vaccination_dose</t>
@@ -954,9 +948,6 @@
     <t>01_T2_43_curate_all_vaccines</t>
   </si>
   <si>
-    <t>04_T2_31_create_study_population_target_cohorts</t>
-  </si>
-  <si>
     <t>D3_study_population_target_cohorts</t>
   </si>
   <si>
@@ -988,6 +979,39 @@
       </rPr>
       <t>condition</t>
     </r>
+  </si>
+  <si>
+    <t>D3_clean_all_vaccines</t>
+  </si>
+  <si>
+    <t>08_T3_12_aggregate_prevalence_vaccination_dose</t>
+  </si>
+  <si>
+    <t>08_T3_11_count_prevalence_vaccination_dose</t>
+  </si>
+  <si>
+    <t>D4_count_vaccination_weekly_prevalence</t>
+  </si>
+  <si>
+    <t>D4_vaccination_weekly_prevalence_aggregated</t>
+  </si>
+  <si>
+    <t>05_T3_41_count_prevalence_indicator</t>
+  </si>
+  <si>
+    <t>D3_vaccine_indicators_dates</t>
+  </si>
+  <si>
+    <t>04_T2_50_create_study_population_target_cohorts</t>
+  </si>
+  <si>
+    <t>04_T2_60_create_vaccine_indicators_dates</t>
+  </si>
+  <si>
+    <t>D4_vaccine_indicators_aggregated</t>
+  </si>
+  <si>
+    <t>D4_count_vaccine_indicators_prevalence</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1110,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1141,6 +1165,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1154,7 +1184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1217,6 +1247,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1531,13 +1566,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
+      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1734,44 +1769,44 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>31</v>
+        <v>249</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -2124,7 +2159,7 @@
     </row>
     <row r="38" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="40" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C38" s="22" t="s">
         <v>93</v>
@@ -2170,173 +2205,166 @@
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="2:8" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="23" t="s">
-        <v>249</v>
-      </c>
-      <c r="C41" s="24" t="s">
+    <row r="41" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="44" t="s">
+        <v>246</v>
+      </c>
+      <c r="C41" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="E41" s="33" t="s">
         <v>248</v>
       </c>
-      <c r="E41" s="34" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>100</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="D42" t="s">
-        <v>45</v>
-      </c>
-      <c r="E42" t="s">
-        <v>102</v>
+    </row>
+    <row r="42" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="E42" s="33" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D43" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="E43" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D44" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="E44" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D45" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="E45" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D46" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
       <c r="E46" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D47" t="s">
         <v>45</v>
       </c>
       <c r="E47" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" t="s">
+        <v>45</v>
+      </c>
+      <c r="E48" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B48" s="21" t="s">
+    <row r="49" spans="2:6" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="C50" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="C48" s="22" t="s">
-        <v>221</v>
-      </c>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21" t="s">
+      <c r="E50" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="F48" s="21"/>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B49" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="F49" s="21"/>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B50" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21" t="s">
-        <v>230</v>
-      </c>
-      <c r="F50" s="21"/>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" s="21" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D51" s="21"/>
       <c r="E51" s="21" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F51" s="21"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B52" t="s">
-        <v>115</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="D52" t="s">
-        <v>105</v>
-      </c>
-      <c r="E52" t="s">
-        <v>113</v>
-      </c>
+      <c r="B52" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="C52" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="F52" s="21"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D53" t="s">
         <v>105</v>
@@ -2346,50 +2374,50 @@
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B54" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="C54" s="22" t="s">
-        <v>233</v>
-      </c>
-      <c r="D54" s="21" t="s">
+      <c r="B54" t="s">
+        <v>117</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D54" t="s">
         <v>105</v>
       </c>
-      <c r="E54" s="21" t="s">
-        <v>227</v>
+      <c r="E54" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" s="21" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D55" s="21" t="s">
         <v>105</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B56" s="29" t="s">
-        <v>235</v>
-      </c>
-      <c r="C56" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="D56" t="s">
-        <v>120</v>
-      </c>
-      <c r="E56" s="13" t="s">
-        <v>121</v>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B56" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E56" s="21" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="57" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B57" s="29" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C57" s="13" t="s">
         <v>119</v>
@@ -2403,7 +2431,7 @@
     </row>
     <row r="58" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B58" s="29" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C58" s="13" t="s">
         <v>119</v>
@@ -2416,22 +2444,22 @@
       </c>
     </row>
     <row r="59" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B59" s="26" t="s">
+      <c r="B59" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D59" t="s">
+        <v>120</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B60" s="26" t="s">
         <v>122</v>
-      </c>
-      <c r="C59" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="D59" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="E59" s="27" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B60" s="30" t="s">
-        <v>123</v>
       </c>
       <c r="C60" s="27" t="s">
         <v>119</v>
@@ -2444,50 +2472,50 @@
       </c>
     </row>
     <row r="61" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B61" s="33" t="s">
+      <c r="B61" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C61" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="D61" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="E61" s="27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B62" s="33" t="s">
+        <v>236</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D62" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="E62" s="22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" s="25" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B63" s="34" t="s">
         <v>238</v>
       </c>
-      <c r="C61" s="22" t="s">
+      <c r="C63" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="D61" s="21" t="s">
+      <c r="D63" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="E61" s="22" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" s="25" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B62" s="34" t="s">
-        <v>240</v>
-      </c>
-      <c r="C62" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="D62" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="E62" s="24" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B63" s="33" t="s">
-        <v>239</v>
-      </c>
-      <c r="C63" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="D63" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="E63" s="22" t="s">
+      <c r="E63" s="24" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="64" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B64" s="33" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C64" s="22" t="s">
         <v>119</v>
@@ -2497,6 +2525,44 @@
       </c>
       <c r="E64" s="22" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B65" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D65" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="E65" s="22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B66" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="C66" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B67" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="C67" s="43" t="s">
+        <v>250</v>
+      </c>
+      <c r="D67" s="42"/>
+      <c r="E67" s="42" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -3744,15 +3810,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
@@ -3762,6 +3819,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3784,14 +3850,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3800,4 +3858,12 @@
     <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
codebooks on vaccination coverage using Toon's method for cohorts (Toon et all, Vaccine 2000)
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -859,9 +859,6 @@
     <t>D4_count_vaccination_prevalence</t>
   </si>
   <si>
-    <t>05_T3_42_aggregate_prevalence_vaccination_dose</t>
-  </si>
-  <si>
     <t>D4_count_events_prevalence</t>
   </si>
   <si>
@@ -996,22 +993,25 @@
     <t>D4_vaccination_weekly_prevalence_aggregated</t>
   </si>
   <si>
-    <t>05_T3_41_count_prevalence_indicator</t>
-  </si>
-  <si>
-    <t>D3_vaccine_indicators_dates</t>
-  </si>
-  <si>
     <t>04_T2_50_create_study_population_target_cohorts</t>
   </si>
   <si>
-    <t>04_T2_60_create_vaccine_indicators_dates</t>
-  </si>
-  <si>
-    <t>D4_vaccine_indicators_aggregated</t>
-  </si>
-  <si>
-    <t>D4_count_vaccine_indicators_prevalence</t>
+    <t>05_T3_41_count_monthly_prevalence_vaccination</t>
+  </si>
+  <si>
+    <t>D5_vaccine_coverage_indicators</t>
+  </si>
+  <si>
+    <t>D5_vaccine_coverage_cohorts</t>
+  </si>
+  <si>
+    <t>06_T4_60_calculate_indicators</t>
+  </si>
+  <si>
+    <t>06_T4_50_calculate_cohort_coverage</t>
+  </si>
+  <si>
+    <t>D4_monthly_prevalence_vaccination_cohorts</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1110,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1171,6 +1171,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1184,7 +1190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1252,6 +1258,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1569,10 +1579,10 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
+      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1769,44 +1779,44 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C13" s="32" t="s">
         <v>244</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>245</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -2159,7 +2169,7 @@
     </row>
     <row r="38" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="40" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C38" s="22" t="s">
         <v>93</v>
@@ -2207,217 +2217,218 @@
     </row>
     <row r="41" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="44" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E41" s="33" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="33" t="s">
-        <v>255</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>257</v>
-      </c>
-      <c r="E42" s="33" t="s">
-        <v>240</v>
+        <v>247</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" t="s">
+        <v>105</v>
+      </c>
+      <c r="E43" t="s">
         <v>100</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="D43" t="s">
-        <v>45</v>
-      </c>
-      <c r="E43" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D44" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="E44" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" t="s">
+        <v>105</v>
+      </c>
+      <c r="E45" t="s">
         <v>106</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D45" t="s">
-        <v>45</v>
-      </c>
-      <c r="E45" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D46" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="E46" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D47" t="s">
         <v>45</v>
       </c>
       <c r="E47" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>113</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="D48" t="s">
-        <v>45</v>
-      </c>
-      <c r="E48" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="F48" s="21"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="21" t="s">
-        <v>259</v>
+        <v>224</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>254</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="D49" s="21"/>
       <c r="E49" s="21" t="s">
-        <v>221</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="F49" s="21"/>
     </row>
     <row r="50" spans="2:6" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B50" s="21" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>223</v>
+        <v>254</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B51" s="21" t="s">
+      <c r="B51" t="s">
+        <v>115</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D51" t="s">
+        <v>105</v>
+      </c>
+      <c r="E51" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>117</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D52" t="s">
+        <v>105</v>
+      </c>
+      <c r="E52" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="C53" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="C51" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="F51" s="21"/>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B52" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="C52" s="22" t="s">
-        <v>227</v>
-      </c>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21" t="s">
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B54" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" s="21" t="s">
         <v>224</v>
-      </c>
-      <c r="F52" s="21"/>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B53" t="s">
-        <v>115</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="D53" t="s">
-        <v>105</v>
-      </c>
-      <c r="E53" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B54" t="s">
-        <v>117</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="D54" t="s">
-        <v>105</v>
-      </c>
-      <c r="E54" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" s="21" t="s">
-        <v>229</v>
+        <v>256</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="D55" s="21" t="s">
-        <v>105</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="D55" s="21"/>
       <c r="E55" s="21" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B56" s="21" t="s">
-        <v>230</v>
-      </c>
-      <c r="C56" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="D56" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="E56" s="21" t="s">
-        <v>225</v>
+        <v>259</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="45" t="s">
+        <v>255</v>
+      </c>
+      <c r="C56" s="46" t="s">
+        <v>257</v>
+      </c>
+      <c r="E56" s="45" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="57" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B57" s="29" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C57" s="13" t="s">
         <v>119</v>
@@ -2431,7 +2442,7 @@
     </row>
     <row r="58" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B58" s="29" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C58" s="13" t="s">
         <v>119</v>
@@ -2445,7 +2456,7 @@
     </row>
     <row r="59" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B59" s="29" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C59" s="13" t="s">
         <v>119</v>
@@ -2487,7 +2498,7 @@
     </row>
     <row r="62" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B62" s="33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C62" s="22" t="s">
         <v>119</v>
@@ -2501,7 +2512,7 @@
     </row>
     <row r="63" spans="2:6" s="25" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B63" s="34" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C63" s="24" t="s">
         <v>119</v>
@@ -2515,7 +2526,7 @@
     </row>
     <row r="64" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B64" s="33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C64" s="22" t="s">
         <v>119</v>
@@ -2529,7 +2540,7 @@
     </row>
     <row r="65" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B65" s="33" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C65" s="22" t="s">
         <v>119</v>
@@ -2543,10 +2554,10 @@
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B66" s="42" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C66" s="43" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D66" s="42"/>
       <c r="E66" s="42" t="s">
@@ -2555,10 +2566,10 @@
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67" s="42" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C67" s="43" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D67" s="42"/>
       <c r="E67" s="42" t="s">
@@ -3810,6 +3821,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
@@ -3819,15 +3839,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3850,6 +3861,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3858,12 +3877,4 @@
     <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
revision during meeting 28 March
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -1110,7 +1110,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1173,7 +1173,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1190,7 +1196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1251,17 +1257,22 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1579,10 +1590,10 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
+      <selection pane="bottomRight" activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1781,7 +1792,7 @@
       <c r="B11" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="43" t="s">
         <v>240</v>
       </c>
       <c r="D11" t="s">
@@ -1795,7 +1806,7 @@
       <c r="B12" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="43" t="s">
         <v>244</v>
       </c>
       <c r="D12" t="s">
@@ -1809,7 +1820,7 @@
       <c r="B13" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="43" t="s">
         <v>244</v>
       </c>
       <c r="D13" t="s">
@@ -1899,7 +1910,7 @@
       <c r="B19" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="24" t="s">
         <v>52</v>
       </c>
       <c r="D19" t="s">
@@ -2167,20 +2178,20 @@
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="40" t="s">
+    <row r="38" spans="2:8" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="44" t="s">
         <v>246</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C38" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="D38" s="21" t="s">
+      <c r="D38" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="41" t="s">
+      <c r="E38" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="H38" s="21" t="s">
+      <c r="H38" s="45" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2215,14 +2226,14 @@
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="2:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="44" t="s">
+    <row r="41" spans="2:8" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="47" t="s">
         <v>245</v>
       </c>
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="42" t="s">
         <v>253</v>
       </c>
-      <c r="E41" s="33" t="s">
+      <c r="E41" s="48" t="s">
         <v>247</v>
       </c>
     </row>
@@ -2310,44 +2321,40 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B48" s="21" t="s">
+    <row r="48" spans="2:8" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="45" t="s">
         <v>223</v>
       </c>
-      <c r="C48" s="22" t="s">
+      <c r="C48" s="42" t="s">
         <v>225</v>
       </c>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21" t="s">
+      <c r="E48" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="F48" s="21"/>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B49" s="21" t="s">
+    </row>
+    <row r="49" spans="2:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="45" t="s">
         <v>224</v>
       </c>
-      <c r="C49" s="22" t="s">
+      <c r="C49" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21" t="s">
+      <c r="E49" s="45" t="s">
         <v>223</v>
       </c>
-      <c r="F49" s="21"/>
-    </row>
-    <row r="50" spans="2:6" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="21" t="s">
+    </row>
+    <row r="50" spans="2:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="49" t="s">
         <v>259</v>
       </c>
-      <c r="C50" s="22" t="s">
+      <c r="C50" s="43" t="s">
         <v>254</v>
       </c>
-      <c r="E50" s="21" t="s">
+      <c r="E50" s="49" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>115</v>
       </c>
@@ -2361,7 +2368,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>117</v>
       </c>
@@ -2375,58 +2382,57 @@
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B53" s="21" t="s">
+    <row r="53" spans="2:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="45" t="s">
         <v>228</v>
       </c>
-      <c r="C53" s="22" t="s">
+      <c r="C53" s="42" t="s">
         <v>230</v>
       </c>
-      <c r="D53" s="21" t="s">
+      <c r="D53" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="E53" s="21" t="s">
+      <c r="E53" s="45" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B54" s="21" t="s">
+    <row r="54" spans="2:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="45" t="s">
         <v>229</v>
       </c>
-      <c r="C54" s="22" t="s">
+      <c r="C54" s="42" t="s">
         <v>231</v>
       </c>
-      <c r="D54" s="21" t="s">
+      <c r="D54" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="E54" s="21" t="s">
+      <c r="E54" s="45" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B55" s="21" t="s">
+    <row r="55" spans="2:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="49" t="s">
         <v>256</v>
       </c>
-      <c r="C55" s="22" t="s">
+      <c r="C55" s="43" t="s">
         <v>258</v>
       </c>
-      <c r="D55" s="21"/>
-      <c r="E55" s="21" t="s">
+      <c r="E55" s="49" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="56" spans="2:6" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="45" t="s">
+    <row r="56" spans="2:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="49" t="s">
         <v>255</v>
       </c>
-      <c r="C56" s="46" t="s">
+      <c r="C56" s="43" t="s">
         <v>257</v>
       </c>
-      <c r="E56" s="45" t="s">
+      <c r="E56" s="49" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="57" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B57" s="29" t="s">
         <v>232</v>
       </c>
@@ -2440,7 +2446,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="58" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B58" s="29" t="s">
         <v>233</v>
       </c>
@@ -2454,7 +2460,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B59" s="29" t="s">
         <v>234</v>
       </c>
@@ -2468,7 +2474,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="60" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B60" s="26" t="s">
         <v>122</v>
       </c>
@@ -2482,7 +2488,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="61" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B61" s="30" t="s">
         <v>123</v>
       </c>
@@ -2496,7 +2502,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="62" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B62" s="33" t="s">
         <v>235</v>
       </c>
@@ -2510,7 +2516,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="63" spans="2:6" s="25" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:5" s="25" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B63" s="34" t="s">
         <v>237</v>
       </c>
@@ -2524,7 +2530,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B64" s="33" t="s">
         <v>236</v>
       </c>
@@ -2553,26 +2559,26 @@
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B66" s="42" t="s">
+      <c r="B66" s="40" t="s">
         <v>251</v>
       </c>
-      <c r="C66" s="43" t="s">
+      <c r="C66" s="41" t="s">
         <v>250</v>
       </c>
-      <c r="D66" s="42"/>
-      <c r="E66" s="42" t="s">
+      <c r="D66" s="40"/>
+      <c r="E66" s="40" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B67" s="42" t="s">
+      <c r="B67" s="40" t="s">
         <v>252</v>
       </c>
-      <c r="C67" s="43" t="s">
+      <c r="C67" s="41" t="s">
         <v>249</v>
       </c>
-      <c r="D67" s="42"/>
-      <c r="E67" s="42" t="s">
+      <c r="D67" s="40"/>
+      <c r="E67" s="40" t="s">
         <v>222</v>
       </c>
     </row>
@@ -3821,15 +3827,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
@@ -3839,6 +3836,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3861,14 +3867,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3877,4 +3875,12 @@
     <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
codebooks fro vaccine coverage
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -939,9 +939,6 @@
     <t>D3_all_clean_vaccines D3_vaccines_curated</t>
   </si>
   <si>
-    <t>Flowchart_criteria_for_doses_all_vaccines</t>
-  </si>
-  <si>
     <t>01_T2_43_curate_all_vaccines</t>
   </si>
   <si>
@@ -996,9 +993,6 @@
     <t>04_T2_50_create_study_population_target_cohorts</t>
   </si>
   <si>
-    <t>05_T3_41_count_monthly_prevalence_vaccination</t>
-  </si>
-  <si>
     <t>D5_vaccine_coverage_indicators</t>
   </si>
   <si>
@@ -1012,6 +1006,12 @@
   </si>
   <si>
     <t>D4_monthly_prevalence_vaccination_cohorts</t>
+  </si>
+  <si>
+    <t>Flowchart_criteria_for_all_vaccines</t>
+  </si>
+  <si>
+    <t>05_T3_70_count_monthly_prevalence_vaccination</t>
   </si>
 </sst>
 </file>
@@ -1590,10 +1590,10 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C55" sqref="C55"/>
+      <selection pane="bottomRight" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1790,7 +1790,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C11" s="43" t="s">
         <v>240</v>
@@ -1807,7 +1807,7 @@
         <v>239</v>
       </c>
       <c r="C12" s="43" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -1818,10 +1818,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C13" s="43" t="s">
         <v>243</v>
-      </c>
-      <c r="C13" s="43" t="s">
-        <v>244</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
@@ -2180,7 +2180,7 @@
     </row>
     <row r="38" spans="2:8" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="44" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C38" s="42" t="s">
         <v>93</v>
@@ -2228,13 +2228,13 @@
     </row>
     <row r="41" spans="2:8" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="47" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C41" s="42" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E41" s="48" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
@@ -2345,10 +2345,10 @@
     </row>
     <row r="50" spans="2:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B50" s="49" t="s">
+        <v>257</v>
+      </c>
+      <c r="C50" s="43" t="s">
         <v>259</v>
-      </c>
-      <c r="C50" s="43" t="s">
-        <v>254</v>
       </c>
       <c r="E50" s="49" t="s">
         <v>221</v>
@@ -2412,24 +2412,24 @@
     </row>
     <row r="55" spans="2:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B55" s="49" t="s">
+        <v>254</v>
+      </c>
+      <c r="C55" s="43" t="s">
         <v>256</v>
       </c>
-      <c r="C55" s="43" t="s">
-        <v>258</v>
-      </c>
       <c r="E55" s="49" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="56" spans="2:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B56" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="C56" s="43" t="s">
         <v>255</v>
       </c>
-      <c r="C56" s="43" t="s">
-        <v>257</v>
-      </c>
       <c r="E56" s="49" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="57" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2560,10 +2560,10 @@
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B66" s="40" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C66" s="41" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D66" s="40"/>
       <c r="E66" s="40" t="s">
@@ -2572,10 +2572,10 @@
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67" s="40" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C67" s="41" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D67" s="40"/>
       <c r="E67" s="40" t="s">
@@ -3576,6 +3576,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -3826,7 +3835,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
@@ -3838,16 +3847,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3866,7 +3874,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3875,12 +3883,4 @@
     <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
delete old shell tables
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\ROC18\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4695FF4-E6C1-45D7-8850-3129B41ECB78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA0C387-220B-4468-9FB0-80416E28E92D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="219">
   <si>
     <t>status</t>
   </si>
@@ -372,12 +372,6 @@
   </si>
   <si>
     <t>Flowchart_exclusion_criteria D3_events_ALL_OUTCOMES D3_Total_study_population D3_covariates_ALL D5_IR_background D5_IR_background_std</t>
-  </si>
-  <si>
-    <t>Table 4</t>
-  </si>
-  <si>
-    <t>Table 5</t>
   </si>
   <si>
     <t>parameter in the table name</t>
@@ -920,7 +914,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -954,12 +948,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1000,7 +988,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1039,35 +1027,29 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1382,13 +1364,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
+      <selection pane="bottomRight" activeCell="B39" sqref="A39:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,7 +1409,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1545,7 +1527,7 @@
       <c r="B8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="25" t="s">
         <v>32</v>
       </c>
       <c r="D8" t="s">
@@ -1562,7 +1544,7 @@
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="25" t="s">
         <v>34</v>
       </c>
       <c r="D9" t="s">
@@ -1576,7 +1558,7 @@
       <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="25" t="s">
         <v>34</v>
       </c>
       <c r="D10" t="s">
@@ -1588,44 +1570,44 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>200</v>
+        <v>205</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>198</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>203</v>
+        <v>197</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>201</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>203</v>
+        <v>216</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>201</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1773,36 +1755,36 @@
       <c r="D23" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="32" t="s">
+      <c r="E23" s="28" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="2:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="37" t="s">
-        <v>205</v>
-      </c>
-      <c r="C24" s="35" t="s">
+    <row r="24" spans="2:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="C24" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="38" t="s">
+      <c r="D24" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="39" t="s">
+      <c r="E24" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="H24" s="38" t="s">
+      <c r="H24" s="34" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="2:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="40" t="s">
+    <row r="25" spans="2:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="36" t="s">
+        <v>202</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>210</v>
+      </c>
+      <c r="E25" s="37" t="s">
         <v>204</v>
-      </c>
-      <c r="C25" s="35" t="s">
-        <v>212</v>
-      </c>
-      <c r="E25" s="41" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -1819,37 +1801,37 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="2:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="38" t="s">
+    <row r="27" spans="2:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="C27" s="31" t="s">
         <v>183</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="E27" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="E27" s="38" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="38" t="s">
+    </row>
+    <row r="28" spans="2:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="C28" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="C28" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="E28" s="38" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="42" t="s">
+      <c r="E28" s="34" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="C29" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="C29" s="36" t="s">
-        <v>219</v>
-      </c>
-      <c r="E29" s="42" t="s">
-        <v>181</v>
+      <c r="E29" s="38" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -1880,59 +1862,59 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="2:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="38" t="s">
+    <row r="32" spans="2:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="D32" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="34" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="34" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="C34" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="E35" s="38" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="24" t="s">
         <v>190</v>
-      </c>
-      <c r="D32" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="E32" s="38" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="38" t="s">
-        <v>189</v>
-      </c>
-      <c r="C33" s="35" t="s">
-        <v>191</v>
-      </c>
-      <c r="D33" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="38" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="42" t="s">
-        <v>214</v>
-      </c>
-      <c r="C34" s="36" t="s">
-        <v>216</v>
-      </c>
-      <c r="E34" s="42" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="42" t="s">
-        <v>213</v>
-      </c>
-      <c r="C35" s="36" t="s">
-        <v>215</v>
-      </c>
-      <c r="E35" s="42" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" s="27" t="s">
-        <v>192</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>79</v>
@@ -1945,8 +1927,8 @@
       </c>
     </row>
     <row r="37" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B37" s="27" t="s">
-        <v>193</v>
+      <c r="B37" s="24" t="s">
+        <v>191</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>79</v>
@@ -1959,8 +1941,8 @@
       </c>
     </row>
     <row r="38" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="27" t="s">
-        <v>194</v>
+      <c r="B38" s="24" t="s">
+        <v>192</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>79</v>
@@ -1973,36 +1955,36 @@
       </c>
     </row>
     <row r="39" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B39" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="25" t="s">
+      <c r="B39" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="C39" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D39" s="26" t="s">
+      <c r="D39" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="E39" s="25" t="s">
+      <c r="E39" s="20" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B40" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="C40" s="25" t="s">
+    <row r="40" spans="2:5" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="C40" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="D40" s="26" t="s">
+      <c r="D40" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="E40" s="25" t="s">
+      <c r="E40" s="22" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="41" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B41" s="30" t="s">
-        <v>195</v>
+      <c r="B41" s="26" t="s">
+        <v>194</v>
       </c>
       <c r="C41" s="20" t="s">
         <v>79</v>
@@ -2014,70 +1996,42 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="2:5" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B42" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="C42" s="22" t="s">
+    <row r="42" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="C42" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D42" s="23" t="s">
+      <c r="D42" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="E42" s="22" t="s">
+      <c r="E42" s="20" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="C43" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E43" s="20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B44" s="30" t="s">
-        <v>198</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E44" s="20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="C45" s="34" t="s">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="C46" s="34" t="s">
-        <v>208</v>
-      </c>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33" t="s">
-        <v>182</v>
+      <c r="C44" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2106,16 +2060,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2123,10 +2077,10 @@
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2134,10 +2088,10 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2145,7 +2099,7 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2153,7 +2107,7 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2161,186 +2115,186 @@
         <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" t="s">
         <v>98</v>
       </c>
-      <c r="B8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" t="s">
-        <v>100</v>
-      </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" t="s">
-        <v>100</v>
-      </c>
       <c r="D9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" t="s">
         <v>98</v>
       </c>
-      <c r="B10" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" t="s">
-        <v>100</v>
-      </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" t="s">
-        <v>100</v>
-      </c>
       <c r="D11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C12" t="s">
-        <v>100</v>
-      </c>
       <c r="D12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" t="s">
-        <v>100</v>
-      </c>
       <c r="D13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" t="s">
         <v>98</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" t="s">
-        <v>100</v>
-      </c>
       <c r="D14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" t="s">
-        <v>100</v>
-      </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" t="s">
         <v>98</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" t="s">
-        <v>100</v>
-      </c>
       <c r="D16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>100</v>
-      </c>
       <c r="D17" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>100</v>
-      </c>
       <c r="D18" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>100</v>
-      </c>
       <c r="D19" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2348,13 +2302,13 @@
         <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2362,13 +2316,13 @@
         <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2376,13 +2330,13 @@
         <v>69</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2390,13 +2344,13 @@
         <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2404,13 +2358,13 @@
         <v>69</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2418,13 +2372,13 @@
         <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2432,640 +2386,640 @@
         <v>69</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B28" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B29" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C29" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C30" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B31" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C31" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B33" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C33" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B34" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C34" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C35" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B36" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C36" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C37" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C38" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B39" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C39" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B40" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C40" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B41" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C41" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B42" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C42" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B43" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C43" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B44" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C44" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B45" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C45" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B46" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C46" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B47" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C47" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B48" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C48" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B49" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C49" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B50" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C50" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B51" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C51" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B52" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C52" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B53" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C53" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B54" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C54" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B55" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C55" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B56" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C56" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B57" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C57" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B58" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C58" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B59" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C59" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B60" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C60" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B61" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C61" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B62" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C62" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B63" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C63" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B64" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C64" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B65" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C65" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B66" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C66" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B67" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C67" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B68" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C68" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B69" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C69" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B70" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C70" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B71" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C71" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B72" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C72" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B73" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C73" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B74" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C74" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B75" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C75" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B76" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C76" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B77" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C77" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B78" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C78" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B79" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C79" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B80" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C80" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B81" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C81" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B82" t="s">
+        <v>176</v>
+      </c>
+      <c r="C82" t="s">
         <v>177</v>
-      </c>
-      <c r="B82" t="s">
-        <v>178</v>
-      </c>
-      <c r="C82" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="B83" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C83" s="18" t="s">
         <v>177</v>
-      </c>
-      <c r="B83" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="C83" s="18" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -3083,6 +3037,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -3333,18 +3299,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>
@@ -3354,6 +3308,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3370,15 +3335,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
cleaned index except setps 05
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20408"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\ROC18\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosgin2\Documents\ROC18\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA0C387-220B-4468-9FB0-80416E28E92D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="211">
   <si>
     <t>status</t>
   </si>
@@ -317,36 +316,12 @@
     <t>04_T2_10_create_total_study_population</t>
   </si>
   <si>
-    <t>D4_study_population D3_vaccines_curated D3_PERSONS D3_covid_episodes</t>
-  </si>
-  <si>
-    <t>D3_study_population_SCRI</t>
-  </si>
-  <si>
-    <t>D3_study_population_cohort</t>
-  </si>
-  <si>
-    <t>04_T2_30_create_study_population_cohort</t>
-  </si>
-  <si>
-    <t>04_T2_40_create_TD_datasets</t>
-  </si>
-  <si>
     <t>condition conceptsets</t>
   </si>
   <si>
     <t>comedication</t>
   </si>
   <si>
-    <t>D4_count_events_windows</t>
-  </si>
-  <si>
-    <t>05_T3_10_count_events_windows</t>
-  </si>
-  <si>
-    <t>D3_study_population_by_window_and_dose D3_events_ALL_OUTCOMES</t>
-  </si>
-  <si>
     <t>g_export/D4-D5 tables</t>
   </si>
   <si>
@@ -665,22 +640,10 @@
     <t xml:space="preserve">E_DM1_AESI </t>
   </si>
   <si>
-    <t>D3_study_population_cohort D3_vaccines_curated</t>
-  </si>
-  <si>
-    <t>D4_count_vaccination_prevalence</t>
-  </si>
-  <si>
     <t>D4_count_events_prevalence</t>
   </si>
   <si>
     <t>D4_events_prevalence_aggregated</t>
-  </si>
-  <si>
-    <t>05_T3_41_count_prevalence_events</t>
-  </si>
-  <si>
-    <t>05_T3_42_aggregate_prevalence_events</t>
   </si>
   <si>
     <t>D3_study_population_cohort D3_events_ALL_OUTCOMES</t>
@@ -748,9 +711,6 @@
     </r>
   </si>
   <si>
-    <t>D3_all_clean_vaccines D3_vaccines_curated</t>
-  </si>
-  <si>
     <t>01_T2_43_curate_all_vaccines</t>
   </si>
   <si>
@@ -790,21 +750,6 @@
     <t>D3_clean_all_vaccines</t>
   </si>
   <si>
-    <t>08_T3_12_aggregate_prevalence_vaccination_dose</t>
-  </si>
-  <si>
-    <t>08_T3_11_count_prevalence_vaccination_dose</t>
-  </si>
-  <si>
-    <t>D4_count_vaccination_weekly_prevalence</t>
-  </si>
-  <si>
-    <t>D4_vaccination_weekly_prevalence_aggregated</t>
-  </si>
-  <si>
-    <t>04_T2_50_create_study_population_target_cohorts</t>
-  </si>
-  <si>
     <t>D5_vaccine_coverage_indicators</t>
   </si>
   <si>
@@ -827,13 +772,43 @@
   </si>
   <si>
     <t>slug</t>
+  </si>
+  <si>
+    <t>D3_clean_all_vaccines D3_vaccines_curated</t>
+  </si>
+  <si>
+    <t>D3_study_population_cohort D3_all_vaccines_curated</t>
+  </si>
+  <si>
+    <t>D4_study_population D3_vaccines_curated D3_PERSONS</t>
+  </si>
+  <si>
+    <t>Flowchart_exclusion_criteria D3_events_ALL_OUTCOMES D3_Total_study_population D5_IR_background D5_IR_background_std</t>
+  </si>
+  <si>
+    <t>05_T3_40_create_counts_person_time_yearly</t>
+  </si>
+  <si>
+    <t>05_T3_41_aggregate_counts_person_time_yearly</t>
+  </si>
+  <si>
+    <t>05_T3_50_count_point_prevalence_events</t>
+  </si>
+  <si>
+    <t>05_T3_51_aggregate_point_prevalence_events</t>
+  </si>
+  <si>
+    <t>05_T3_60_count_period_prevalence_events</t>
+  </si>
+  <si>
+    <t>05_T3_61_aggregate_period_prevalence_events</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -863,12 +838,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -914,7 +883,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -959,12 +928,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -988,7 +951,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1001,9 +964,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1022,37 +985,31 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1363,27 +1320,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B39" sqref="A39:XFD40"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23:B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.85546875" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="5" width="86.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.88671875" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="86.33203125" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1409,10 +1366,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1429,7 +1386,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
@@ -1443,7 +1400,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1460,7 +1417,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1480,7 +1437,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1500,7 +1457,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1520,14 +1477,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="24" t="s">
         <v>32</v>
       </c>
       <c r="D8" t="s">
@@ -1537,14 +1494,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D9" t="s">
@@ -1554,11 +1511,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D10" t="s">
@@ -1568,49 +1525,49 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>198</v>
+        <v>192</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>186</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>201</v>
+        <v>185</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>188</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>201</v>
+        <v>198</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>188</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>37</v>
       </c>
@@ -1624,7 +1581,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1641,7 +1598,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1658,7 +1615,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>46</v>
       </c>
@@ -1672,7 +1629,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
         <v>47</v>
       </c>
@@ -1686,11 +1643,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="21" t="s">
         <v>52</v>
       </c>
       <c r="D19" t="s">
@@ -1700,7 +1657,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>53</v>
       </c>
@@ -1714,7 +1671,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
         <v>57</v>
       </c>
@@ -1731,7 +1688,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>61</v>
       </c>
@@ -1742,296 +1699,257 @@
         <v>11</v>
       </c>
       <c r="E22" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23" s="30" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="2:8" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
+    <row r="24" spans="2:8" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="27" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="27"/>
+    </row>
+    <row r="30" spans="2:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="E31" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="33" t="s">
-        <v>203</v>
-      </c>
-      <c r="C24" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="H24" s="34" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="36" t="s">
-        <v>202</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="E25" s="37" t="s">
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="34" t="s">
+        <v>194</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="E35" s="34" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="34" t="s">
+        <v>193</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="E36" s="34" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B37" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B38" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" t="s">
+        <v>72</v>
+      </c>
+      <c r="E38" s="13" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="13" t="s">
+    <row r="39" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B39" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="C39" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D26" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="D39" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="34" t="s">
+      <c r="E39" s="13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B40" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C40" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" s="22" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B41" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="E27" s="34" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="34" t="s">
+      <c r="C41" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B42" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C42" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B43" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="E28" s="34" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="38" t="s">
-        <v>215</v>
-      </c>
-      <c r="C29" s="32" t="s">
-        <v>217</v>
-      </c>
-      <c r="E29" s="38" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C43" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E43" s="20" t="s">
         <v>73</v>
-      </c>
-      <c r="E30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D31" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="34" t="s">
-        <v>186</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>188</v>
-      </c>
-      <c r="D32" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E32" s="34" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="34" t="s">
-        <v>187</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>189</v>
-      </c>
-      <c r="D33" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="34" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="38" t="s">
-        <v>212</v>
-      </c>
-      <c r="C34" s="32" t="s">
-        <v>214</v>
-      </c>
-      <c r="E34" s="38" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="38" t="s">
-        <v>211</v>
-      </c>
-      <c r="C35" s="32" t="s">
-        <v>213</v>
-      </c>
-      <c r="E35" s="38" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D36" t="s">
-        <v>80</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B37" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D37" t="s">
-        <v>80</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" t="s">
-        <v>80</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B39" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="C39" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E39" s="20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B40" s="27" t="s">
-        <v>195</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="D40" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="E40" s="22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B41" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E41" s="20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B42" s="26" t="s">
-        <v>196</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="E42" s="20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="29" t="s">
-        <v>208</v>
-      </c>
-      <c r="C43" s="30" t="s">
-        <v>207</v>
-      </c>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="29" t="s">
-        <v>209</v>
-      </c>
-      <c r="C44" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2041,7 +1959,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2051,975 +1969,975 @@
       <selection pane="bottomRight" activeCell="A8" sqref="A8:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.42578125" customWidth="1"/>
-    <col min="3" max="3" width="53.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.44140625" customWidth="1"/>
+    <col min="3" max="3" width="53.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" t="s">
         <v>92</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C17" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C10" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="C18" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="C11" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="C19" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
         <v>102</v>
       </c>
-      <c r="C12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="C20" t="s">
         <v>103</v>
       </c>
-      <c r="C13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="D20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" t="s">
         <v>104</v>
       </c>
-      <c r="C14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="C21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C15" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="C22" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
         <v>106</v>
       </c>
-      <c r="C16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B17" s="16" t="s">
+      <c r="C23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" s="16" t="s">
+      <c r="C24" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" s="16" t="s">
+      <c r="C25" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20" t="s">
-        <v>110</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="C26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" t="s">
         <v>111</v>
       </c>
-      <c r="D20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" t="s">
-        <v>112</v>
-      </c>
-      <c r="C21" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="C27" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" t="s">
         <v>113</v>
       </c>
-      <c r="C22" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" t="s">
         <v>114</v>
       </c>
-      <c r="C23" t="s">
-        <v>111</v>
-      </c>
-      <c r="D23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="C29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" t="s">
         <v>115</v>
       </c>
-      <c r="C24" t="s">
-        <v>111</v>
-      </c>
-      <c r="D24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="C30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" t="s">
         <v>116</v>
       </c>
-      <c r="C25" t="s">
-        <v>111</v>
-      </c>
-      <c r="D25" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="C31" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" t="s">
         <v>117</v>
       </c>
-      <c r="C26" t="s">
-        <v>111</v>
-      </c>
-      <c r="D26" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="C32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" t="s">
         <v>118</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C33" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" t="s">
         <v>119</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="C35" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" t="s">
         <v>121</v>
       </c>
-      <c r="C28" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="C36" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" t="s">
         <v>122</v>
       </c>
-      <c r="C29" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C37" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" t="s">
         <v>123</v>
       </c>
-      <c r="C30" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="C38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B39" t="s">
         <v>124</v>
       </c>
-      <c r="C31" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="C39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" t="s">
         <v>125</v>
       </c>
-      <c r="C32" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="C40" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" t="s">
         <v>126</v>
       </c>
-      <c r="C33" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C41" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B42" t="s">
         <v>127</v>
       </c>
-      <c r="C34" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="C42" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43" t="s">
         <v>128</v>
       </c>
-      <c r="C35" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="C43" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" t="s">
         <v>129</v>
       </c>
-      <c r="C36" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="C44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45" t="s">
         <v>130</v>
       </c>
-      <c r="C37" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="C45" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" t="s">
         <v>131</v>
       </c>
-      <c r="C38" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="C46" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B47" t="s">
         <v>132</v>
       </c>
-      <c r="C39" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="C47" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B48" t="s">
         <v>133</v>
       </c>
-      <c r="C40" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="C48" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B49" t="s">
         <v>134</v>
       </c>
-      <c r="C41" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="C49" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B50" t="s">
         <v>135</v>
       </c>
-      <c r="C42" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="C50" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51" t="s">
         <v>136</v>
       </c>
-      <c r="C43" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="C51" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52" t="s">
         <v>137</v>
       </c>
-      <c r="C44" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="C52" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B53" t="s">
         <v>138</v>
       </c>
-      <c r="C45" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="C53" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B54" t="s">
         <v>139</v>
       </c>
-      <c r="C46" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="C54" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B55" t="s">
         <v>140</v>
       </c>
-      <c r="C47" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B48" t="s">
+      <c r="C55" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" t="s">
         <v>141</v>
       </c>
-      <c r="C48" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="C56" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" t="s">
         <v>142</v>
       </c>
-      <c r="C49" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="C57" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" t="s">
         <v>143</v>
       </c>
-      <c r="C50" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="C58" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59" t="s">
         <v>144</v>
       </c>
-      <c r="C51" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="C59" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" t="s">
         <v>145</v>
       </c>
-      <c r="C52" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="C60" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B61" t="s">
         <v>146</v>
       </c>
-      <c r="C53" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="C61" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B62" t="s">
         <v>147</v>
       </c>
-      <c r="C54" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="C62" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B63" t="s">
         <v>148</v>
       </c>
-      <c r="C55" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="C63" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B64" t="s">
         <v>149</v>
       </c>
-      <c r="C56" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="C64" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B65" t="s">
         <v>150</v>
       </c>
-      <c r="C57" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="C65" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B66" t="s">
         <v>151</v>
       </c>
-      <c r="C58" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="C66" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B67" t="s">
         <v>152</v>
       </c>
-      <c r="C59" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="C67" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B68" t="s">
         <v>153</v>
       </c>
-      <c r="C60" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="C68" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B69" t="s">
         <v>154</v>
       </c>
-      <c r="C61" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B62" t="s">
+      <c r="C69" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B70" t="s">
         <v>155</v>
       </c>
-      <c r="C62" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="C70" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B71" t="s">
         <v>156</v>
       </c>
-      <c r="C63" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B64" t="s">
+      <c r="C71" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B72" t="s">
         <v>157</v>
       </c>
-      <c r="C64" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B65" t="s">
+      <c r="C72" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B73" t="s">
         <v>158</v>
       </c>
-      <c r="C65" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B66" t="s">
+      <c r="C73" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B74" t="s">
         <v>159</v>
       </c>
-      <c r="C66" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B67" t="s">
+      <c r="C74" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B75" t="s">
         <v>160</v>
       </c>
-      <c r="C67" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B68" t="s">
+      <c r="C75" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B76" t="s">
         <v>161</v>
       </c>
-      <c r="C68" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B69" t="s">
+      <c r="C76" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B77" t="s">
         <v>162</v>
       </c>
-      <c r="C69" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B70" t="s">
+      <c r="C77" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B78" t="s">
         <v>163</v>
       </c>
-      <c r="C70" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B71" t="s">
+      <c r="C78" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B79" t="s">
         <v>164</v>
       </c>
-      <c r="C71" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B72" t="s">
+      <c r="C79" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B80" t="s">
         <v>165</v>
       </c>
-      <c r="C72" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B73" t="s">
+      <c r="C80" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B81" t="s">
         <v>166</v>
       </c>
-      <c r="C73" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B74" t="s">
+      <c r="C81" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C74" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B75" t="s">
+      <c r="B82" t="s">
         <v>168</v>
       </c>
-      <c r="C75" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B76" t="s">
+      <c r="C82" t="s">
         <v>169</v>
       </c>
-      <c r="C76" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B77" t="s">
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B83" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="C77" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B78" t="s">
-        <v>171</v>
-      </c>
-      <c r="C78" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B79" t="s">
-        <v>172</v>
-      </c>
-      <c r="C79" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B80" t="s">
-        <v>173</v>
-      </c>
-      <c r="C80" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B81" t="s">
-        <v>174</v>
-      </c>
-      <c r="C81" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B82" t="s">
-        <v>176</v>
-      </c>
-      <c r="C82" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="B83" s="18" t="s">
-        <v>178</v>
-      </c>
       <c r="C83" s="18" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3037,18 +2955,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -3299,6 +3205,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>
@@ -3308,17 +3226,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3335,4 +3242,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated index with correct linkage
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20408"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosgin2\Documents\ROC18\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\ROC18\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC969247-701D-4844-8FFF-839EF1A9F0C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="226">
   <si>
     <t>status</t>
   </si>
@@ -282,25 +283,6 @@
     <t>g_intermediate/TD</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>QC_all_components_</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>OUTCOME</t>
-    </r>
-  </si>
-  <si>
     <t>03_T2_40_create_components</t>
   </si>
   <si>
@@ -325,18 +307,9 @@
     <t>g_export/D4-D5 tables</t>
   </si>
   <si>
-    <t>D4_persontime_background_aggregated</t>
-  </si>
-  <si>
-    <t>D5_IR_background</t>
-  </si>
-  <si>
     <t>06_T4_10_create_D5_IR_background</t>
   </si>
   <si>
-    <t>D5_IR_background_std</t>
-  </si>
-  <si>
     <t>06_T4_20_create_D5_IR_background_std</t>
   </si>
   <si>
@@ -346,9 +319,6 @@
     <t>g_export/Dummy tables</t>
   </si>
   <si>
-    <t>Flowchart_exclusion_criteria D3_events_ALL_OUTCOMES D3_Total_study_population D3_covariates_ALL D5_IR_background D5_IR_background_std</t>
-  </si>
-  <si>
     <t>parameter in the table name</t>
   </si>
   <si>
@@ -638,21 +608,6 @@
   </si>
   <si>
     <t xml:space="preserve">E_DM1_AESI </t>
-  </si>
-  <si>
-    <t>D4_count_events_prevalence</t>
-  </si>
-  <si>
-    <t>D4_events_prevalence_aggregated</t>
-  </si>
-  <si>
-    <t>D3_study_population_cohort D3_events_ALL_OUTCOMES</t>
-  </si>
-  <si>
-    <t>D5_Pre_background</t>
-  </si>
-  <si>
-    <t>D5_Pre_background_std</t>
   </si>
   <si>
     <t>06_T4_30_create_D5_Pre_background</t>
@@ -717,8 +672,65 @@
     <t>D3_study_population_target_cohorts</t>
   </si>
   <si>
+    <t>D3_clean_all_vaccines</t>
+  </si>
+  <si>
+    <t>D5_vaccine_coverage_indicators</t>
+  </si>
+  <si>
+    <t>D5_vaccine_coverage_cohorts</t>
+  </si>
+  <si>
+    <t>06_T4_60_calculate_indicators</t>
+  </si>
+  <si>
+    <t>06_T4_50_calculate_cohort_coverage</t>
+  </si>
+  <si>
+    <t>D4_monthly_prevalence_vaccination_cohorts</t>
+  </si>
+  <si>
+    <t>Flowchart_criteria_for_all_vaccines</t>
+  </si>
+  <si>
+    <t>05_T3_70_count_monthly_prevalence_vaccination</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>D3_clean_all_vaccines D3_vaccines_curated</t>
+  </si>
+  <si>
+    <t>05_T3_40_create_counts_person_time_yearly</t>
+  </si>
+  <si>
+    <t>05_T3_41_aggregate_counts_person_time_yearly</t>
+  </si>
+  <si>
+    <t>05_T3_50_count_point_prevalence_events</t>
+  </si>
+  <si>
+    <t>05_T3_51_aggregate_point_prevalence_events</t>
+  </si>
+  <si>
+    <t>05_T3_60_count_period_prevalence_events</t>
+  </si>
+  <si>
+    <t>05_T3_61_aggregate_period_prevalence_events</t>
+  </si>
+  <si>
+    <t>D4_study_population D3_PERSONS</t>
+  </si>
+  <si>
+    <t>04_T2_40_create_TD_datasets</t>
+  </si>
+  <si>
+    <t>04_T2_43_create_TD_covariates</t>
+  </si>
+  <si>
     <r>
-      <t>D3_TD_variable_</t>
+      <t>D3_TD_</t>
     </r>
     <r>
       <rPr>
@@ -728,12 +740,30 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
+      <t>all</t>
+    </r>
+  </si>
+  <si>
+    <t>D3_TD_covariates_complete</t>
+  </si>
+  <si>
+    <r>
+      <t>D4_study_population D3_TD_</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF444444"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
       <t>condition</t>
     </r>
   </si>
   <si>
     <r>
-      <t>D3_study_population_cohort D3_TD_variable_</t>
+      <t>QC_all_components_</t>
     </r>
     <r>
       <rPr>
@@ -741,74 +771,110 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+      </rPr>
+      <t>OUTCOME</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D4_study_population D3_TD_</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF444444"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>condition</t>
+      <t>OUTCOME</t>
     </r>
   </si>
   <si>
-    <t>D3_clean_all_vaccines</t>
-  </si>
-  <si>
-    <t>D5_vaccine_coverage_indicators</t>
-  </si>
-  <si>
-    <t>D5_vaccine_coverage_cohorts</t>
-  </si>
-  <si>
-    <t>06_T4_60_calculate_indicators</t>
-  </si>
-  <si>
-    <t>06_T4_50_calculate_cohort_coverage</t>
-  </si>
-  <si>
-    <t>D4_monthly_prevalence_vaccination_cohorts</t>
-  </si>
-  <si>
-    <t>Flowchart_criteria_for_all_vaccines</t>
-  </si>
-  <si>
-    <t>05_T3_70_count_monthly_prevalence_vaccination</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>D3_clean_all_vaccines D3_vaccines_curated</t>
-  </si>
-  <si>
-    <t>D3_study_population_cohort D3_all_vaccines_curated</t>
-  </si>
-  <si>
-    <t>D4_study_population D3_vaccines_curated D3_PERSONS</t>
-  </si>
-  <si>
-    <t>Flowchart_exclusion_criteria D3_events_ALL_OUTCOMES D3_Total_study_population D5_IR_background D5_IR_background_std</t>
-  </si>
-  <si>
-    <t>05_T3_40_create_counts_person_time_yearly</t>
-  </si>
-  <si>
-    <t>05_T3_41_aggregate_counts_person_time_yearly</t>
-  </si>
-  <si>
-    <t>05_T3_50_count_point_prevalence_events</t>
-  </si>
-  <si>
-    <t>05_T3_51_aggregate_point_prevalence_events</t>
-  </si>
-  <si>
-    <t>05_T3_60_count_period_prevalence_events</t>
-  </si>
-  <si>
-    <t>05_T3_61_aggregate_period_prevalence_events</t>
+    <t>04_T2_44_create_TD_events</t>
+  </si>
+  <si>
+    <t>D3_TD_events_complete</t>
+  </si>
+  <si>
+    <t>04_T2_50_create_study_population_target_cohorts</t>
+  </si>
+  <si>
+    <t>D3_Total_study_population D3_events_ALL_OUTCOMES</t>
+  </si>
+  <si>
+    <t>D4_counts_persontime_yearly</t>
+  </si>
+  <si>
+    <t>D4_counts_persontime_yearly_aggregated</t>
+  </si>
+  <si>
+    <t>D3_Total_study_population D3_TD_events_complete</t>
+  </si>
+  <si>
+    <t>D4_count_events_point_prevalence</t>
+  </si>
+  <si>
+    <t>D4_events_point_prevalence_aggregated</t>
+  </si>
+  <si>
+    <t>D4_count_events_period_prevalence</t>
+  </si>
+  <si>
+    <t>D4_events_period_prevalence_aggregated</t>
+  </si>
+  <si>
+    <r>
+      <t>D4_monthly_prevalence_vaccination_</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cohorts</t>
+    </r>
+  </si>
+  <si>
+    <t>D3_study_population_target_cohorts D3_all_vaccines_curated</t>
+  </si>
+  <si>
+    <t>D5_IR_yearly</t>
+  </si>
+  <si>
+    <t>D5_IR_yearly_std</t>
+  </si>
+  <si>
+    <t>06_T4_20_create_D5_Pre_background</t>
+  </si>
+  <si>
+    <t>D4_events_point_prevalence_aggregated D4_events_period_prevalence_aggregated</t>
+  </si>
+  <si>
+    <t>D5_Pre_point_background</t>
+  </si>
+  <si>
+    <t>D5_Pre_period_background</t>
+  </si>
+  <si>
+    <t>D5_Pre_point_background_std</t>
+  </si>
+  <si>
+    <t>D5_Pre_period_background_std</t>
+  </si>
+  <si>
+    <t>Flowchart_exclusion_criteria D3_events_ALL_OUTCOMES D3_Total_study_population D3_TD_covariates_complete D3_study_population_target_cohorts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -878,12 +944,19 @@
     <font>
       <i/>
       <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -938,6 +1011,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -951,7 +1030,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1001,15 +1080,22 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1320,27 +1406,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B23" sqref="B23:B26"/>
+      <selection pane="bottomRight" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.88671875" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
-    <col min="5" max="5" width="86.33203125" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.7109375" customWidth="1"/>
+    <col min="3" max="3" width="46.5703125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="86.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1366,10 +1452,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1386,7 +1472,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
@@ -1400,7 +1486,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1417,7 +1503,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1437,11 +1523,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="33" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="12" t="s">
@@ -1457,11 +1543,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="33" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="12" t="s">
@@ -1477,7 +1563,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1494,7 +1580,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1511,7 +1597,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
@@ -1525,49 +1611,49 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="34" t="s">
+        <v>186</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>37</v>
       </c>
@@ -1581,7 +1667,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1598,7 +1684,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1615,7 +1701,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>46</v>
       </c>
@@ -1629,7 +1715,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>47</v>
       </c>
@@ -1643,7 +1729,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>51</v>
       </c>
@@ -1657,7 +1743,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>53</v>
       </c>
@@ -1671,285 +1757,405 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="9" t="s">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="D21" t="s">
         <v>58</v>
-      </c>
-      <c r="D21" t="s">
-        <v>59</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>50</v>
       </c>
       <c r="H21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+      <c r="C22" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
       </c>
       <c r="E22" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="38" t="s">
+        <v>205</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="30" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="29" t="s">
+      <c r="H25" s="29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="38" t="s">
+        <v>208</v>
+      </c>
+      <c r="C27" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="C23" s="27" t="s">
-        <v>205</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="H23" s="30" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="32" t="s">
-        <v>189</v>
-      </c>
-      <c r="C24" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="E24" s="33" t="s">
+      <c r="D27" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="39" t="s">
+        <v>209</v>
+      </c>
+      <c r="C28" s="27" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="30" t="s">
+      <c r="D28" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="31" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="34" t="s">
+        <v>211</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="C31" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="34" t="s">
+        <v>214</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="40" t="s">
+        <v>217</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="40" t="s">
+        <v>218</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="34" t="s">
+        <v>221</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="C37" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="34" t="s">
+        <v>223</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="29" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="E40" s="32" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="E41" s="32" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" t="s">
+        <v>68</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" t="s">
+        <v>68</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" s="40" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="E44" s="24" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B45" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="C25" s="27" t="s">
-        <v>207</v>
-      </c>
-      <c r="E25" s="30" t="s">
+      <c r="C45" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="26" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="30" t="s">
+      <c r="C46" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B47" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="C26" s="27" t="s">
-        <v>208</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="27" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="27" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="27"/>
-    </row>
-    <row r="30" spans="2:8" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="34" t="s">
-        <v>197</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="E30" s="34" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
+      <c r="C47" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="D47" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>69</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="30" t="s">
+      <c r="E47" s="20" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="C33" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="D33" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="30" t="s">
-        <v>175</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>177</v>
-      </c>
-      <c r="D34" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E34" s="30" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="34" t="s">
-        <v>194</v>
-      </c>
-      <c r="C35" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="E35" s="34" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="34" t="s">
-        <v>193</v>
-      </c>
-      <c r="C36" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="E36" s="34" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B37" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D37" t="s">
-        <v>72</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B38" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D38" t="s">
-        <v>72</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B39" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D39" t="s">
-        <v>72</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B40" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" s="22" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B41" s="26" t="s">
-        <v>183</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D41" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B42" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E42" s="20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B43" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="C43" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="E43" s="20" t="s">
-        <v>73</v>
+      <c r="C48" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -1959,985 +2165,985 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8:B9"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.44140625" customWidth="1"/>
-    <col min="3" max="3" width="53.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="3" max="3" width="53.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B8" t="s">
         <v>84</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C8" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="D8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="C10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="C15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="C16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="C17" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="3" t="s">
+      <c r="C18" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C14" t="s">
-        <v>90</v>
-      </c>
-      <c r="D14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="C19" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
         <v>97</v>
       </c>
-      <c r="C15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="C20" t="s">
         <v>98</v>
       </c>
-      <c r="C16" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" s="16" t="s">
+      <c r="D20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B18" s="16" t="s">
+      <c r="C21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B19" s="16" t="s">
+      <c r="C22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="C23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
         <v>103</v>
       </c>
-      <c r="D20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C21" t="s">
-        <v>103</v>
-      </c>
-      <c r="D21" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C22" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C26" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" t="s">
         <v>106</v>
       </c>
-      <c r="C23" t="s">
-        <v>103</v>
-      </c>
-      <c r="D23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="C27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" t="s">
         <v>108</v>
       </c>
-      <c r="C25" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="C28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" t="s">
         <v>109</v>
       </c>
-      <c r="C26" t="s">
-        <v>103</v>
-      </c>
-      <c r="D26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="C29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" t="s">
         <v>110</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" t="s">
         <v>111</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="C32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" t="s">
         <v>113</v>
       </c>
-      <c r="C28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="C33" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" t="s">
         <v>114</v>
       </c>
-      <c r="C29" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C34" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" t="s">
         <v>115</v>
       </c>
-      <c r="C30" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="C35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" t="s">
         <v>116</v>
       </c>
-      <c r="C31" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="C36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" t="s">
         <v>117</v>
       </c>
-      <c r="C32" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="C37" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" t="s">
         <v>118</v>
       </c>
-      <c r="C33" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" t="s">
         <v>119</v>
       </c>
-      <c r="C34" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="C39" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" t="s">
         <v>120</v>
       </c>
-      <c r="C35" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="C40" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" t="s">
         <v>121</v>
       </c>
-      <c r="C36" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="C41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B42" t="s">
         <v>122</v>
       </c>
-      <c r="C37" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="C42" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43" t="s">
         <v>123</v>
       </c>
-      <c r="C38" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="C43" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" t="s">
         <v>124</v>
       </c>
-      <c r="C39" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="C44" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" t="s">
         <v>125</v>
       </c>
-      <c r="C40" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="C45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" t="s">
         <v>126</v>
       </c>
-      <c r="C41" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="C46" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" t="s">
         <v>127</v>
       </c>
-      <c r="C42" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="C47" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B48" t="s">
         <v>128</v>
       </c>
-      <c r="C43" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="C48" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B49" t="s">
         <v>129</v>
       </c>
-      <c r="C44" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="C49" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" t="s">
         <v>130</v>
       </c>
-      <c r="C45" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="C50" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51" t="s">
         <v>131</v>
       </c>
-      <c r="C46" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="C51" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" t="s">
         <v>132</v>
       </c>
-      <c r="C47" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B48" t="s">
+      <c r="C52" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" t="s">
         <v>133</v>
       </c>
-      <c r="C48" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="C53" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" t="s">
         <v>134</v>
       </c>
-      <c r="C49" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="C54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B55" t="s">
         <v>135</v>
       </c>
-      <c r="C50" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="C55" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" t="s">
         <v>136</v>
       </c>
-      <c r="C51" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="C56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B57" t="s">
         <v>137</v>
       </c>
-      <c r="C52" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="C57" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B58" t="s">
         <v>138</v>
       </c>
-      <c r="C53" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="C58" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" t="s">
         <v>139</v>
       </c>
-      <c r="C54" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="C59" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B60" t="s">
         <v>140</v>
       </c>
-      <c r="C55" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="C60" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" t="s">
         <v>141</v>
       </c>
-      <c r="C56" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="C61" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B62" t="s">
         <v>142</v>
       </c>
-      <c r="C57" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="C62" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63" t="s">
         <v>143</v>
       </c>
-      <c r="C58" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="C63" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B64" t="s">
         <v>144</v>
       </c>
-      <c r="C59" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="C64" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B65" t="s">
         <v>145</v>
       </c>
-      <c r="C60" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="C65" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B66" t="s">
         <v>146</v>
       </c>
-      <c r="C61" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B62" t="s">
+      <c r="C66" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B67" t="s">
         <v>147</v>
       </c>
-      <c r="C62" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="C67" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B68" t="s">
         <v>148</v>
       </c>
-      <c r="C63" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B64" t="s">
+      <c r="C68" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B69" t="s">
         <v>149</v>
       </c>
-      <c r="C64" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B65" t="s">
+      <c r="C69" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B70" t="s">
         <v>150</v>
       </c>
-      <c r="C65" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B66" t="s">
+      <c r="C70" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B71" t="s">
         <v>151</v>
       </c>
-      <c r="C66" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B67" t="s">
+      <c r="C71" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B72" t="s">
         <v>152</v>
       </c>
-      <c r="C67" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B68" t="s">
+      <c r="C72" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B73" t="s">
         <v>153</v>
       </c>
-      <c r="C68" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B69" t="s">
+      <c r="C73" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B74" t="s">
         <v>154</v>
       </c>
-      <c r="C69" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B70" t="s">
+      <c r="C74" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B75" t="s">
         <v>155</v>
       </c>
-      <c r="C70" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B71" t="s">
+      <c r="C75" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B76" t="s">
         <v>156</v>
       </c>
-      <c r="C71" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B72" t="s">
+      <c r="C76" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B77" t="s">
         <v>157</v>
       </c>
-      <c r="C72" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B73" t="s">
+      <c r="C77" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B78" t="s">
         <v>158</v>
       </c>
-      <c r="C73" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B74" t="s">
+      <c r="C78" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B79" t="s">
         <v>159</v>
       </c>
-      <c r="C74" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B75" t="s">
+      <c r="C79" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B80" t="s">
         <v>160</v>
       </c>
-      <c r="C75" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B76" t="s">
+      <c r="C80" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B81" t="s">
         <v>161</v>
       </c>
-      <c r="C76" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B77" t="s">
+      <c r="C81" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C77" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B78" t="s">
+      <c r="B82" t="s">
         <v>163</v>
       </c>
-      <c r="C78" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B79" t="s">
+      <c r="C82" t="s">
         <v>164</v>
       </c>
-      <c r="C79" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B80" t="s">
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B83" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="C80" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B81" t="s">
-        <v>166</v>
-      </c>
-      <c r="C81" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B82" t="s">
-        <v>168</v>
-      </c>
-      <c r="C82" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="B83" s="18" t="s">
-        <v>170</v>
-      </c>
       <c r="C83" s="18" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2955,6 +3161,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -3205,18 +3423,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>
@@ -3226,6 +3432,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3242,21 +3465,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated index, diagram, website and parameters
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\ROC18\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC969247-701D-4844-8FFF-839EF1A9F0C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00F87CD-9AE3-49C5-B8FF-46240498DF0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="225">
   <si>
     <t>status</t>
   </si>
@@ -310,9 +310,6 @@
     <t>06_T4_10_create_D5_IR_background</t>
   </si>
   <si>
-    <t>06_T4_20_create_D5_IR_background_std</t>
-  </si>
-  <si>
     <t>07_T5_10_final_tables</t>
   </si>
   <si>
@@ -608,12 +605,6 @@
   </si>
   <si>
     <t xml:space="preserve">E_DM1_AESI </t>
-  </si>
-  <si>
-    <t>06_T4_30_create_D5_Pre_background</t>
-  </si>
-  <si>
-    <t>06_T4_40_create_D5_Pre_background_std</t>
   </si>
   <si>
     <t>Table_1_flowchart</t>
@@ -868,6 +859,12 @@
   </si>
   <si>
     <t>Flowchart_exclusion_criteria D3_events_ALL_OUTCOMES D3_Total_study_population D3_TD_covariates_complete D3_study_population_target_cohorts</t>
+  </si>
+  <si>
+    <t>06_T4_21_create_D5_Pre_background_std</t>
+  </si>
+  <si>
+    <t>06_T4_11_create_D5_IR_background_std</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1094,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1410,10 +1418,10 @@
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E50" sqref="E50"/>
+      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,7 +1460,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1613,44 +1621,44 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" s="28" t="s">
         <v>175</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>178</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="34" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1759,7 +1767,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="35" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>57</v>
@@ -1785,15 +1793,15 @@
         <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="37" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D23" s="29" t="s">
         <v>56</v>
@@ -1807,16 +1815,16 @@
     </row>
     <row r="24" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="37" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D24" s="29" t="s">
         <v>56</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H24" s="29" t="s">
         <v>62</v>
@@ -1824,16 +1832,16 @@
     </row>
     <row r="25" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="38" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D25" s="29" t="s">
         <v>56</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H25" s="29" t="s">
         <v>62</v>
@@ -1841,10 +1849,10 @@
     </row>
     <row r="26" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="36" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D26" s="29" t="s">
         <v>11</v>
@@ -1858,16 +1866,16 @@
     </row>
     <row r="27" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="38" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D27" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H27" s="29" t="s">
         <v>62</v>
@@ -1875,88 +1883,88 @@
     </row>
     <row r="28" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="39" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D28" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="34" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D29" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="34" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D30" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="34" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D31" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="34" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D32" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="32" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E33" s="32" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="40" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>65</v>
@@ -1965,200 +1973,203 @@
         <v>64</v>
       </c>
       <c r="E34" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="40" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>66</v>
+        <v>224</v>
       </c>
       <c r="D35" t="s">
         <v>64</v>
       </c>
       <c r="E35" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="34" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D36" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="34" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D37" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="C38" s="27" t="s">
         <v>223</v>
-      </c>
-      <c r="C38" s="27" t="s">
-        <v>166</v>
       </c>
       <c r="D38" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="34" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>167</v>
+        <v>223</v>
       </c>
       <c r="D39" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="40" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="E40" s="32" t="s">
         <v>182</v>
-      </c>
-      <c r="C40" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="E40" s="32" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="41" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="32" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E41" s="32" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="23" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C42" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" t="s">
         <v>67</v>
       </c>
-      <c r="D42" t="s">
-        <v>68</v>
-      </c>
       <c r="E42" s="13" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="23" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C43" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" t="s">
         <v>67</v>
       </c>
-      <c r="D43" t="s">
-        <v>68</v>
-      </c>
       <c r="E43" s="13" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="2:5" s="40" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="41" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C44" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="40" t="s">
-        <v>68</v>
-      </c>
       <c r="E44" s="24" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="25" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C45" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D45" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="19" t="s">
-        <v>68</v>
-      </c>
       <c r="E45" s="20" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="46" spans="2:5" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="26" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C46" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="D46" s="22" t="s">
-        <v>68</v>
-      </c>
       <c r="E46" s="13" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="25" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C47" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D47" s="19" t="s">
-        <v>68</v>
-      </c>
       <c r="E47" s="20" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="48" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="25" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C48" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D48" s="19" t="s">
-        <v>68</v>
-      </c>
       <c r="E48" s="20" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2184,16 +2195,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2201,10 +2212,10 @@
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
         <v>73</v>
-      </c>
-      <c r="D2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2212,10 +2223,10 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
         <v>75</v>
-      </c>
-      <c r="D3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2223,7 +2234,7 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2231,7 +2242,7 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2239,186 +2250,186 @@
         <v>59</v>
       </c>
       <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
         <v>79</v>
-      </c>
-      <c r="D6" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
         <v>81</v>
-      </c>
-      <c r="B7" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
         <v>83</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>84</v>
       </c>
-      <c r="C8" t="s">
-        <v>85</v>
-      </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2426,13 +2437,13 @@
         <v>63</v>
       </c>
       <c r="B20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" t="s">
         <v>97</v>
       </c>
-      <c r="C20" t="s">
-        <v>98</v>
-      </c>
       <c r="D20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2440,13 +2451,13 @@
         <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2454,13 +2465,13 @@
         <v>63</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2468,13 +2479,13 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2482,13 +2493,13 @@
         <v>63</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2496,13 +2507,13 @@
         <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2510,640 +2521,640 @@
         <v>63</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" t="s">
         <v>105</v>
       </c>
-      <c r="B27" t="s">
-        <v>106</v>
-      </c>
       <c r="C27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B42" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B44" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B46" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B49" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B50" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B51" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C52" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B53" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C53" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C54" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B55" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B56" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C56" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B57" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B59" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C59" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B60" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C60" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B61" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C61" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B62" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C62" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B63" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C63" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B64" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B65" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C65" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B66" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C66" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B67" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C67" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B68" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B69" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C69" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B70" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C70" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B71" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B72" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C72" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B73" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B74" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C74" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B75" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C75" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B76" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C76" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B77" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C77" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B78" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C78" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B79" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C79" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B80" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C80" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B81" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C81" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B82" t="s">
         <v>162</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>163</v>
-      </c>
-      <c r="C82" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -3161,18 +3172,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -3423,6 +3422,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>
@@ -3432,23 +3443,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3465,4 +3459,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
codebooks of calculation of vaccine coverage
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20408"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\ROC18\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosgin2\Documents\ROC18\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00F87CD-9AE3-49C5-B8FF-46240498DF0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="223">
   <si>
     <t>status</t>
   </si>
@@ -666,13 +665,7 @@
     <t>D3_clean_all_vaccines</t>
   </si>
   <si>
-    <t>D5_vaccine_coverage_indicators</t>
-  </si>
-  <si>
     <t>D5_vaccine_coverage_cohorts</t>
-  </si>
-  <si>
-    <t>06_T4_60_calculate_indicators</t>
   </si>
   <si>
     <t>06_T4_50_calculate_cohort_coverage</t>
@@ -870,7 +863,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1092,7 +1085,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1414,27 +1407,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C38" sqref="C38"/>
+      <selection pane="bottomRight" activeCell="B41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="44.7109375" customWidth="1"/>
-    <col min="3" max="3" width="46.5703125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="5" width="86.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.6640625" customWidth="1"/>
+    <col min="3" max="3" width="46.5546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="86.33203125" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1460,10 +1453,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1480,7 +1473,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
@@ -1494,7 +1487,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1511,7 +1504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1531,7 +1524,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1551,7 +1544,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1571,7 +1564,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1588,7 +1581,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1605,7 +1598,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
@@ -1619,7 +1612,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>177</v>
       </c>
@@ -1633,7 +1626,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>172</v>
       </c>
@@ -1644,12 +1637,12 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="34" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C13" s="28" t="s">
         <v>175</v>
@@ -1658,10 +1651,10 @@
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>37</v>
       </c>
@@ -1675,7 +1668,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1692,7 +1685,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1709,7 +1702,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>46</v>
       </c>
@@ -1723,7 +1716,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
         <v>47</v>
       </c>
@@ -1737,7 +1730,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
         <v>51</v>
       </c>
@@ -1751,7 +1744,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>53</v>
       </c>
@@ -1765,9 +1758,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>57</v>
@@ -1782,7 +1775,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>60</v>
       </c>
@@ -1793,15 +1786,15 @@
         <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="37" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D23" s="29" t="s">
         <v>56</v>
@@ -1813,46 +1806,46 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="37" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D24" s="29" t="s">
         <v>56</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H24" s="29" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="38" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D25" s="29" t="s">
         <v>56</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H25" s="29" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="36" t="s">
         <v>176</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D26" s="29" t="s">
         <v>11</v>
@@ -1864,107 +1857,107 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="38" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D27" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H27" s="29" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28" s="39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D28" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B29" s="34" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D29" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E29" s="29" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="34" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="34" t="s">
-        <v>209</v>
-      </c>
       <c r="C30" s="27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D30" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E30" s="29" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="34" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="34" t="s">
-        <v>210</v>
-      </c>
       <c r="C31" s="27" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D31" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="34" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D32" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E32" s="29" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="32" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="33" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="32" t="s">
+      <c r="C33" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="40" t="s">
         <v>212</v>
-      </c>
-      <c r="C33" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="E33" s="32" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="40" t="s">
-        <v>214</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>65</v>
@@ -1973,104 +1966,107 @@
         <v>64</v>
       </c>
       <c r="E34" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="40" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D35" t="s">
         <v>64</v>
       </c>
       <c r="E35" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="34" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D36" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E36" s="29" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="34" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="34" t="s">
-        <v>219</v>
-      </c>
       <c r="C37" s="27" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D37" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="34" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D38" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="34" t="s">
+        <v>219</v>
+      </c>
+      <c r="C39" s="27" t="s">
         <v>221</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>223</v>
       </c>
       <c r="D39" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="C40" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="C40" s="28" t="s">
-        <v>181</v>
-      </c>
       <c r="E40" s="32" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="C41" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="E41" s="32" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B41" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B42" s="23" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C42" s="13" t="s">
         <v>66</v>
@@ -2079,68 +2075,68 @@
         <v>67</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="C43" s="13" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" s="40" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B43" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="E43" s="13" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" s="40" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B44" s="41" t="s">
-        <v>167</v>
-      </c>
-      <c r="C44" s="24" t="s">
+      <c r="E43" s="24" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B44" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="C44" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D44" s="40" t="s">
+      <c r="D44" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="E44" s="24" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B45" s="25" t="s">
-        <v>168</v>
-      </c>
-      <c r="C45" s="20" t="s">
+      <c r="E44" s="20" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" s="22" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B45" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="C45" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="19" t="s">
+      <c r="D45" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="E45" s="20" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B46" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="C46" s="21" t="s">
+      <c r="E45" s="13" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B46" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="C46" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D46" s="22" t="s">
+      <c r="D46" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="E46" s="13" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E46" s="20" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B47" s="25" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C47" s="20" t="s">
         <v>66</v>
@@ -2149,21 +2145,7 @@
         <v>67</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2176,7 +2158,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2186,14 +2168,14 @@
       <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.42578125" customWidth="1"/>
-    <col min="3" max="3" width="53.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.44140625" customWidth="1"/>
+    <col min="3" max="3" width="53.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>68</v>
       </c>
@@ -2207,7 +2189,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -2218,7 +2200,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -2229,7 +2211,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -2237,7 +2219,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -2245,7 +2227,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>59</v>
       </c>
@@ -2256,7 +2238,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>80</v>
       </c>
@@ -2264,7 +2246,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>82</v>
       </c>
@@ -2278,7 +2260,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>82</v>
       </c>
@@ -2292,7 +2274,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>82</v>
       </c>
@@ -2306,7 +2288,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>82</v>
       </c>
@@ -2320,7 +2302,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>82</v>
       </c>
@@ -2334,7 +2316,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>82</v>
       </c>
@@ -2348,7 +2330,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>82</v>
       </c>
@@ -2362,7 +2344,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>82</v>
       </c>
@@ -2376,7 +2358,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>82</v>
       </c>
@@ -2390,7 +2372,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>82</v>
       </c>
@@ -2404,7 +2386,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>82</v>
       </c>
@@ -2418,7 +2400,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>82</v>
       </c>
@@ -2432,7 +2414,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>63</v>
       </c>
@@ -2446,7 +2428,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
@@ -2460,7 +2442,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>63</v>
       </c>
@@ -2474,7 +2456,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>63</v>
       </c>
@@ -2488,7 +2470,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
@@ -2502,7 +2484,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>63</v>
       </c>
@@ -2516,7 +2498,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
@@ -2530,7 +2512,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>104</v>
       </c>
@@ -2541,7 +2523,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>104</v>
       </c>
@@ -2552,7 +2534,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>104</v>
       </c>
@@ -2563,7 +2545,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>104</v>
       </c>
@@ -2574,7 +2556,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>104</v>
       </c>
@@ -2585,7 +2567,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>104</v>
       </c>
@@ -2596,7 +2578,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>104</v>
       </c>
@@ -2607,7 +2589,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>104</v>
       </c>
@@ -2618,7 +2600,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>104</v>
       </c>
@@ -2629,7 +2611,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>104</v>
       </c>
@@ -2640,7 +2622,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>104</v>
       </c>
@@ -2651,7 +2633,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>104</v>
       </c>
@@ -2662,7 +2644,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>104</v>
       </c>
@@ -2673,7 +2655,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>104</v>
       </c>
@@ -2684,7 +2666,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>104</v>
       </c>
@@ -2695,7 +2677,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>104</v>
       </c>
@@ -2706,7 +2688,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>104</v>
       </c>
@@ -2717,7 +2699,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>104</v>
       </c>
@@ -2728,7 +2710,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>104</v>
       </c>
@@ -2739,7 +2721,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>104</v>
       </c>
@@ -2750,7 +2732,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>104</v>
       </c>
@@ -2761,7 +2743,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>104</v>
       </c>
@@ -2772,7 +2754,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>104</v>
       </c>
@@ -2783,7 +2765,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>104</v>
       </c>
@@ -2794,7 +2776,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>104</v>
       </c>
@@ -2805,7 +2787,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>104</v>
       </c>
@@ -2816,7 +2798,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>104</v>
       </c>
@@ -2827,7 +2809,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>104</v>
       </c>
@@ -2838,7 +2820,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>104</v>
       </c>
@@ -2849,7 +2831,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>104</v>
       </c>
@@ -2860,7 +2842,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>104</v>
       </c>
@@ -2871,7 +2853,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>104</v>
       </c>
@@ -2882,7 +2864,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>104</v>
       </c>
@@ -2893,7 +2875,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>104</v>
       </c>
@@ -2904,7 +2886,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>104</v>
       </c>
@@ -2915,7 +2897,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>104</v>
       </c>
@@ -2926,7 +2908,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>104</v>
       </c>
@@ -2937,7 +2919,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>104</v>
       </c>
@@ -2948,7 +2930,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>104</v>
       </c>
@@ -2959,7 +2941,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>104</v>
       </c>
@@ -2970,7 +2952,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>104</v>
       </c>
@@ -2981,7 +2963,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>104</v>
       </c>
@@ -2992,7 +2974,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>104</v>
       </c>
@@ -3003,7 +2985,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>104</v>
       </c>
@@ -3014,7 +2996,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>104</v>
       </c>
@@ -3025,7 +3007,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>104</v>
       </c>
@@ -3036,7 +3018,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>104</v>
       </c>
@@ -3047,7 +3029,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>104</v>
       </c>
@@ -3058,7 +3040,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>104</v>
       </c>
@@ -3069,7 +3051,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>104</v>
       </c>
@@ -3080,7 +3062,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>104</v>
       </c>
@@ -3091,7 +3073,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>104</v>
       </c>
@@ -3102,7 +3084,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>104</v>
       </c>
@@ -3113,7 +3095,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>104</v>
       </c>
@@ -3124,7 +3106,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>104</v>
       </c>
@@ -3135,7 +3117,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>161</v>
       </c>
@@ -3146,7 +3128,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="17" t="s">
         <v>161</v>
       </c>
@@ -3163,12 +3145,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3423,21 +3408,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3462,18 +3453,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
introduced parameter for cohorts
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="238">
   <si>
     <t>status</t>
   </si>
@@ -808,6 +808,45 @@
     <t>D4_events_period_prevalence_aggregated</t>
   </si>
   <si>
+    <t>D3_study_population_target_cohorts D3_all_vaccines_curated</t>
+  </si>
+  <si>
+    <t>D5_IR_yearly</t>
+  </si>
+  <si>
+    <t>D5_IR_yearly_std</t>
+  </si>
+  <si>
+    <t>06_T4_20_create_D5_Pre_background</t>
+  </si>
+  <si>
+    <t>D4_events_point_prevalence_aggregated D4_events_period_prevalence_aggregated</t>
+  </si>
+  <si>
+    <t>D5_Pre_point_background</t>
+  </si>
+  <si>
+    <t>D5_Pre_period_background</t>
+  </si>
+  <si>
+    <t>D5_Pre_point_background_std</t>
+  </si>
+  <si>
+    <t>D5_Pre_period_background_std</t>
+  </si>
+  <si>
+    <t>Flowchart_exclusion_criteria D3_events_ALL_OUTCOMES D3_Total_study_population D3_TD_covariates_complete D3_study_population_target_cohorts</t>
+  </si>
+  <si>
+    <t>06_T4_21_create_D5_Pre_background_std</t>
+  </si>
+  <si>
+    <t>06_T4_11_create_D5_IR_background_std</t>
+  </si>
+  <si>
+    <t>cohort</t>
+  </si>
+  <si>
     <r>
       <t>D4_monthly_prevalence_vaccination_</t>
     </r>
@@ -820,44 +859,50 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>cohorts</t>
+      <t>cohort</t>
     </r>
   </si>
   <si>
-    <t>D3_study_population_target_cohorts D3_all_vaccines_curated</t>
-  </si>
-  <si>
-    <t>D5_IR_yearly</t>
-  </si>
-  <si>
-    <t>D5_IR_yearly_std</t>
-  </si>
-  <si>
-    <t>06_T4_20_create_D5_Pre_background</t>
-  </si>
-  <si>
-    <t>D4_events_point_prevalence_aggregated D4_events_period_prevalence_aggregated</t>
-  </si>
-  <si>
-    <t>D5_Pre_point_background</t>
-  </si>
-  <si>
-    <t>D5_Pre_period_background</t>
-  </si>
-  <si>
-    <t>D5_Pre_point_background_std</t>
-  </si>
-  <si>
-    <t>D5_Pre_period_background_std</t>
-  </si>
-  <si>
-    <t>Flowchart_exclusion_criteria D3_events_ALL_OUTCOMES D3_Total_study_population D3_TD_covariates_complete D3_study_population_target_cohorts</t>
-  </si>
-  <si>
-    <t>06_T4_21_create_D5_Pre_background_std</t>
-  </si>
-  <si>
-    <t>06_T4_11_create_D5_IR_background_std</t>
+    <t>list_of_cohorts_for_coverage</t>
+  </si>
+  <si>
+    <t>birth12</t>
+  </si>
+  <si>
+    <t>birth24</t>
+  </si>
+  <si>
+    <t>birth15</t>
+  </si>
+  <si>
+    <t>adolescence</t>
+  </si>
+  <si>
+    <t>covid_vacc</t>
+  </si>
+  <si>
+    <t>seasonal2017</t>
+  </si>
+  <si>
+    <t>seasonal2018</t>
+  </si>
+  <si>
+    <t>seasonal2019</t>
+  </si>
+  <si>
+    <t>seasonal2020</t>
+  </si>
+  <si>
+    <t>seasonal2021</t>
+  </si>
+  <si>
+    <t>seasonal2022</t>
+  </si>
+  <si>
+    <t>seasonal2023</t>
+  </si>
+  <si>
+    <t>11_design_parameters</t>
   </si>
 </sst>
 </file>
@@ -1410,11 +1455,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B41" sqref="A41:XFD41"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1946,18 +1991,18 @@
     </row>
     <row r="33" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="32" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="C33" s="28" t="s">
         <v>182</v>
       </c>
       <c r="E33" s="32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="40" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>65</v>
@@ -1971,10 +2016,10 @@
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="40" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D35" t="s">
         <v>64</v>
@@ -1985,58 +2030,58 @@
     </row>
     <row r="36" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D36" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="37" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D37" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="38" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D38" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="34" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D39" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="40" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.3">
@@ -2061,7 +2106,7 @@
         <v>67</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2075,7 +2120,7 @@
         <v>67</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="43" spans="2:5" s="40" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -2089,7 +2134,7 @@
         <v>67</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2103,7 +2148,7 @@
         <v>67</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="45" spans="2:5" s="22" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -2117,7 +2162,7 @@
         <v>67</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2131,7 +2176,7 @@
         <v>67</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -2145,7 +2190,7 @@
         <v>67</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -2159,13 +2204,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3106,7 +3151,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>104</v>
       </c>
@@ -3117,7 +3162,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>161</v>
       </c>
@@ -3128,7 +3173,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="17" t="s">
         <v>161</v>
       </c>
@@ -3139,8 +3184,182 @@
         <v>163</v>
       </c>
     </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B85" t="s">
+        <v>225</v>
+      </c>
+      <c r="C85" t="s">
+        <v>224</v>
+      </c>
+      <c r="D85" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B86" t="s">
+        <v>226</v>
+      </c>
+      <c r="C86" t="s">
+        <v>224</v>
+      </c>
+      <c r="D86" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B87" t="s">
+        <v>227</v>
+      </c>
+      <c r="C87" t="s">
+        <v>224</v>
+      </c>
+      <c r="D87" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B88" t="s">
+        <v>228</v>
+      </c>
+      <c r="C88" t="s">
+        <v>224</v>
+      </c>
+      <c r="D88" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B89" t="s">
+        <v>229</v>
+      </c>
+      <c r="C89" t="s">
+        <v>224</v>
+      </c>
+      <c r="D89" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B90" t="s">
+        <v>230</v>
+      </c>
+      <c r="C90" t="s">
+        <v>224</v>
+      </c>
+      <c r="D90" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B91" t="s">
+        <v>231</v>
+      </c>
+      <c r="C91" t="s">
+        <v>224</v>
+      </c>
+      <c r="D91" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B92" t="s">
+        <v>232</v>
+      </c>
+      <c r="C92" t="s">
+        <v>224</v>
+      </c>
+      <c r="D92" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B93" t="s">
+        <v>233</v>
+      </c>
+      <c r="C93" t="s">
+        <v>224</v>
+      </c>
+      <c r="D93" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B94" t="s">
+        <v>234</v>
+      </c>
+      <c r="C94" t="s">
+        <v>224</v>
+      </c>
+      <c r="D94" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B95" t="s">
+        <v>235</v>
+      </c>
+      <c r="C95" t="s">
+        <v>224</v>
+      </c>
+      <c r="D95" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B96" t="s">
+        <v>236</v>
+      </c>
+      <c r="C96" t="s">
+        <v>224</v>
+      </c>
+      <c r="D96" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D97" t="s">
+        <v>237</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3157,6 +3376,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -3407,15 +3635,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
   <ds:schemaRefs>
@@ -3434,6 +3653,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3450,12 +3677,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Remove final tables not produced anymore from index
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20408"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosgin2\Documents\ROC18\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\ROC18\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE1C503-A3DC-440D-B47C-7B7F9B6B8335}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="235">
   <si>
     <t>status</t>
   </si>
@@ -615,18 +616,6 @@
     <t>Table_3_population</t>
   </si>
   <si>
-    <t>Table_4_vaccination_prevalence</t>
-  </si>
-  <si>
-    <t>Table_6_events_prevalence</t>
-  </si>
-  <si>
-    <t>Table_5_events_IR</t>
-  </si>
-  <si>
-    <t>Table_7_components</t>
-  </si>
-  <si>
     <t>D3_all_vaccines_curated</t>
   </si>
   <si>
@@ -904,11 +893,14 @@
   <si>
     <t>11_design_parameters</t>
   </si>
+  <si>
+    <t>Flowchart_exclusion_criteria D3_events_ALL_OUTCOMES D3_Total_study_population D3_TD_all D3_study_population_target_cohorts</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1130,7 +1122,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1452,27 +1444,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomRight" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="44.6640625" customWidth="1"/>
-    <col min="3" max="3" width="46.5546875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
-    <col min="5" max="5" width="86.33203125" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.7109375" customWidth="1"/>
+    <col min="3" max="3" width="46.5703125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="86.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1498,10 +1490,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1518,7 +1510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
@@ -1532,7 +1524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1549,7 +1541,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1569,7 +1561,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1589,7 +1581,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1609,7 +1601,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1626,7 +1618,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1643,7 +1635,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
@@ -1657,49 +1649,49 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="34" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D13" t="s">
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>37</v>
       </c>
@@ -1713,7 +1705,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1730,7 +1722,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1747,7 +1739,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>46</v>
       </c>
@@ -1761,7 +1753,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>47</v>
       </c>
@@ -1775,7 +1767,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>51</v>
       </c>
@@ -1789,7 +1781,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>53</v>
       </c>
@@ -1803,9 +1795,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="35" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>57</v>
@@ -1820,7 +1812,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>60</v>
       </c>
@@ -1831,15 +1823,15 @@
         <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="37" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D23" s="29" t="s">
         <v>56</v>
@@ -1851,46 +1843,46 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="37" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D24" s="29" t="s">
         <v>56</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="H24" s="29" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="38" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D25" s="29" t="s">
         <v>56</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H25" s="29" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="36" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D26" s="29" t="s">
         <v>11</v>
@@ -1902,107 +1894,107 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="38" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D27" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H27" s="29" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="39" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D28" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="34" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D29" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="34" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D30" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="34" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D31" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E31" s="29" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="34" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="34" t="s">
-        <v>209</v>
-      </c>
       <c r="C32" s="27" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D32" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="32" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E33" s="32" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="40" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>65</v>
@@ -2011,91 +2003,91 @@
         <v>64</v>
       </c>
       <c r="E34" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="40" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D35" t="s">
         <v>64</v>
       </c>
       <c r="E35" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="34" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D36" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="34" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D37" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="34" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D38" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E38" s="29" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="34" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="34" t="s">
-        <v>218</v>
-      </c>
       <c r="C39" s="27" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D39" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="32" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E40" s="32" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" s="23" t="s">
         <v>165</v>
       </c>
@@ -2106,10 +2098,10 @@
         <v>67</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="23" t="s">
         <v>166</v>
       </c>
@@ -2120,10 +2112,10 @@
         <v>67</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" s="40" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" s="40" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="41" t="s">
         <v>167</v>
       </c>
@@ -2134,64 +2126,31 @@
         <v>67</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B44" s="25" t="s">
-        <v>168</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E44" s="20" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" s="22" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B45" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D45" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B46" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B47" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E47" s="20" t="s">
-        <v>219</v>
-      </c>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="25"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="20"/>
+    </row>
+    <row r="45" spans="2:5" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="26"/>
+      <c r="C45" s="21"/>
+      <c r="E45" s="13"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="25"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="20"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="25"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="20"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
@@ -2203,24 +2162,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.44140625" customWidth="1"/>
-    <col min="3" max="3" width="53.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="3" max="3" width="53.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>68</v>
       </c>
@@ -2234,7 +2193,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -2245,7 +2204,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -2256,7 +2215,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -2264,7 +2223,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -2272,7 +2231,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>59</v>
       </c>
@@ -2283,7 +2242,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>80</v>
       </c>
@@ -2291,7 +2250,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>82</v>
       </c>
@@ -2305,7 +2264,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>82</v>
       </c>
@@ -2319,7 +2278,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>82</v>
       </c>
@@ -2333,7 +2292,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>82</v>
       </c>
@@ -2347,7 +2306,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>82</v>
       </c>
@@ -2361,7 +2320,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>82</v>
       </c>
@@ -2375,7 +2334,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>82</v>
       </c>
@@ -2389,7 +2348,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>82</v>
       </c>
@@ -2403,7 +2362,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>82</v>
       </c>
@@ -2417,7 +2376,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>82</v>
       </c>
@@ -2431,7 +2390,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>82</v>
       </c>
@@ -2445,7 +2404,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>82</v>
       </c>
@@ -2459,7 +2418,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>63</v>
       </c>
@@ -2473,7 +2432,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
@@ -2487,7 +2446,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>63</v>
       </c>
@@ -2501,7 +2460,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>63</v>
       </c>
@@ -2515,7 +2474,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
@@ -2529,7 +2488,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>63</v>
       </c>
@@ -2543,7 +2502,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
@@ -2557,7 +2516,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>104</v>
       </c>
@@ -2568,7 +2527,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>104</v>
       </c>
@@ -2579,7 +2538,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>104</v>
       </c>
@@ -2590,7 +2549,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>104</v>
       </c>
@@ -2601,7 +2560,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>104</v>
       </c>
@@ -2612,7 +2571,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>104</v>
       </c>
@@ -2623,7 +2582,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>104</v>
       </c>
@@ -2634,7 +2593,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>104</v>
       </c>
@@ -2645,7 +2604,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>104</v>
       </c>
@@ -2656,7 +2615,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>104</v>
       </c>
@@ -2667,7 +2626,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>104</v>
       </c>
@@ -2678,7 +2637,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>104</v>
       </c>
@@ -2689,7 +2648,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>104</v>
       </c>
@@ -2700,7 +2659,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>104</v>
       </c>
@@ -2711,7 +2670,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>104</v>
       </c>
@@ -2722,7 +2681,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>104</v>
       </c>
@@ -2733,7 +2692,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>104</v>
       </c>
@@ -2744,7 +2703,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>104</v>
       </c>
@@ -2755,7 +2714,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>104</v>
       </c>
@@ -2766,7 +2725,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>104</v>
       </c>
@@ -2777,7 +2736,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>104</v>
       </c>
@@ -2788,7 +2747,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>104</v>
       </c>
@@ -2799,7 +2758,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>104</v>
       </c>
@@ -2810,7 +2769,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>104</v>
       </c>
@@ -2821,7 +2780,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>104</v>
       </c>
@@ -2832,7 +2791,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>104</v>
       </c>
@@ -2843,7 +2802,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>104</v>
       </c>
@@ -2854,7 +2813,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>104</v>
       </c>
@@ -2865,7 +2824,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>104</v>
       </c>
@@ -2876,7 +2835,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>104</v>
       </c>
@@ -2887,7 +2846,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>104</v>
       </c>
@@ -2898,7 +2857,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>104</v>
       </c>
@@ -2909,7 +2868,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>104</v>
       </c>
@@ -2920,7 +2879,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>104</v>
       </c>
@@ -2931,7 +2890,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>104</v>
       </c>
@@ -2942,7 +2901,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>104</v>
       </c>
@@ -2953,7 +2912,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>104</v>
       </c>
@@ -2964,7 +2923,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>104</v>
       </c>
@@ -2975,7 +2934,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>104</v>
       </c>
@@ -2986,7 +2945,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>104</v>
       </c>
@@ -2997,7 +2956,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>104</v>
       </c>
@@ -3008,7 +2967,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>104</v>
       </c>
@@ -3019,7 +2978,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>104</v>
       </c>
@@ -3030,7 +2989,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>104</v>
       </c>
@@ -3041,7 +3000,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>104</v>
       </c>
@@ -3052,7 +3011,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>104</v>
       </c>
@@ -3063,7 +3022,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>104</v>
       </c>
@@ -3074,7 +3033,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>104</v>
       </c>
@@ -3085,7 +3044,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>104</v>
       </c>
@@ -3096,7 +3055,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>104</v>
       </c>
@@ -3107,7 +3066,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>104</v>
       </c>
@@ -3118,7 +3077,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>104</v>
       </c>
@@ -3129,7 +3088,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>104</v>
       </c>
@@ -3140,7 +3099,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>104</v>
       </c>
@@ -3151,7 +3110,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>104</v>
       </c>
@@ -3162,7 +3121,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>161</v>
       </c>
@@ -3173,7 +3132,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
         <v>161</v>
       </c>
@@ -3184,177 +3143,177 @@
         <v>163</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B85" t="s">
+        <v>221</v>
+      </c>
+      <c r="C85" t="s">
+        <v>220</v>
+      </c>
+      <c r="D85" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B86" t="s">
         <v>222</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C86" t="s">
+        <v>220</v>
+      </c>
+      <c r="D86" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B87" t="s">
+        <v>223</v>
+      </c>
+      <c r="C87" t="s">
+        <v>220</v>
+      </c>
+      <c r="D87" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B88" t="s">
+        <v>224</v>
+      </c>
+      <c r="C88" t="s">
+        <v>220</v>
+      </c>
+      <c r="D88" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B89" t="s">
         <v>225</v>
       </c>
-      <c r="C85" t="s">
-        <v>224</v>
-      </c>
-      <c r="D85" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B86" t="s">
+      <c r="C89" t="s">
+        <v>220</v>
+      </c>
+      <c r="D89" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B90" t="s">
         <v>226</v>
       </c>
-      <c r="C86" t="s">
-        <v>224</v>
-      </c>
-      <c r="D86" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B87" t="s">
+      <c r="C90" t="s">
+        <v>220</v>
+      </c>
+      <c r="D90" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B91" t="s">
         <v>227</v>
       </c>
-      <c r="C87" t="s">
-        <v>224</v>
-      </c>
-      <c r="D87" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B88" t="s">
+      <c r="C91" t="s">
+        <v>220</v>
+      </c>
+      <c r="D91" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B92" t="s">
         <v>228</v>
       </c>
-      <c r="C88" t="s">
-        <v>224</v>
-      </c>
-      <c r="D88" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B89" t="s">
+      <c r="C92" t="s">
+        <v>220</v>
+      </c>
+      <c r="D92" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B93" t="s">
         <v>229</v>
       </c>
-      <c r="C89" t="s">
-        <v>224</v>
-      </c>
-      <c r="D89" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B90" t="s">
+      <c r="C93" t="s">
+        <v>220</v>
+      </c>
+      <c r="D93" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B94" t="s">
         <v>230</v>
       </c>
-      <c r="C90" t="s">
-        <v>224</v>
-      </c>
-      <c r="D90" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B91" t="s">
+      <c r="C94" t="s">
+        <v>220</v>
+      </c>
+      <c r="D94" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B95" t="s">
         <v>231</v>
       </c>
-      <c r="C91" t="s">
-        <v>224</v>
-      </c>
-      <c r="D91" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B92" t="s">
+      <c r="C95" t="s">
+        <v>220</v>
+      </c>
+      <c r="D95" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B96" t="s">
         <v>232</v>
       </c>
-      <c r="C92" t="s">
-        <v>224</v>
-      </c>
-      <c r="D92" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B93" t="s">
+      <c r="C96" t="s">
+        <v>220</v>
+      </c>
+      <c r="D96" t="s">
         <v>233</v>
       </c>
-      <c r="C93" t="s">
-        <v>224</v>
-      </c>
-      <c r="D93" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B94" t="s">
-        <v>234</v>
-      </c>
-      <c r="C94" t="s">
-        <v>224</v>
-      </c>
-      <c r="D94" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B95" t="s">
-        <v>235</v>
-      </c>
-      <c r="C95" t="s">
-        <v>224</v>
-      </c>
-      <c r="D95" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B96" t="s">
-        <v>236</v>
-      </c>
-      <c r="C96" t="s">
-        <v>224</v>
-      </c>
-      <c r="D96" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D97" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3376,15 +3335,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -3635,6 +3585,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
   <ds:schemaRefs>
@@ -3653,14 +3612,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3677,4 +3628,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
corrected typo in index
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20408"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\ROC18\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosgin2\Documents\ROC18\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE1C503-A3DC-440D-B47C-7B7F9B6B8335}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -660,9 +659,6 @@
     <t>06_T4_50_calculate_cohort_coverage</t>
   </si>
   <si>
-    <t>D4_monthly_prevalence_vaccination_cohorts</t>
-  </si>
-  <si>
     <t>Flowchart_criteria_for_all_vaccines</t>
   </si>
   <si>
@@ -896,11 +892,14 @@
   <si>
     <t>Flowchart_exclusion_criteria D3_events_ALL_OUTCOMES D3_Total_study_population D3_TD_all D3_study_population_target_cohorts</t>
   </si>
+  <si>
+    <t>D4_monthly_prevalence_vaccination_cohort</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1122,7 +1121,7 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1444,27 +1443,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E42" sqref="E42"/>
+      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="44.7109375" customWidth="1"/>
-    <col min="3" max="3" width="46.5703125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="5" width="86.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.6640625" customWidth="1"/>
+    <col min="3" max="3" width="46.5546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="86.33203125" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1490,10 +1489,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1510,7 +1509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
@@ -1524,7 +1523,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1541,7 +1540,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1561,7 +1560,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1581,7 +1580,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1601,7 +1600,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1618,7 +1617,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1635,7 +1634,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>35</v>
       </c>
@@ -1649,7 +1648,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>173</v>
       </c>
@@ -1663,7 +1662,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>168</v>
       </c>
@@ -1674,12 +1673,12 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C13" s="28" t="s">
         <v>171</v>
@@ -1688,10 +1687,10 @@
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>37</v>
       </c>
@@ -1705,7 +1704,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1722,7 +1721,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1739,7 +1738,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>46</v>
       </c>
@@ -1753,7 +1752,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
         <v>47</v>
       </c>
@@ -1767,7 +1766,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
         <v>51</v>
       </c>
@@ -1781,7 +1780,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>53</v>
       </c>
@@ -1795,9 +1794,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>57</v>
@@ -1812,7 +1811,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>60</v>
       </c>
@@ -1823,15 +1822,15 @@
         <v>11</v>
       </c>
       <c r="E22" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="C23" s="27" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="37" t="s">
-        <v>190</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>188</v>
       </c>
       <c r="D23" s="29" t="s">
         <v>56</v>
@@ -1843,46 +1842,46 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="37" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D24" s="29" t="s">
         <v>56</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H24" s="29" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="38" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D25" s="29" t="s">
         <v>56</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H25" s="29" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="2:8" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="36" t="s">
         <v>172</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D26" s="29" t="s">
         <v>11</v>
@@ -1894,107 +1893,107 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D27" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H27" s="29" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28" s="39" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D28" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B29" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D29" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B30" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D30" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D31" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D32" s="29" t="s">
         <v>45</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E33" s="32" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="40" t="s">
         <v>206</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="40" t="s">
-        <v>207</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>65</v>
@@ -2003,80 +2002,80 @@
         <v>64</v>
       </c>
       <c r="E34" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="40" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D35" t="s">
         <v>64</v>
       </c>
       <c r="E35" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D36" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D37" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="34" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D38" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="34" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D39" s="29" t="s">
         <v>64</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" s="32" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="32" t="s">
         <v>174</v>
       </c>
@@ -2084,10 +2083,10 @@
         <v>175</v>
       </c>
       <c r="E40" s="32" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B41" s="23" t="s">
         <v>165</v>
       </c>
@@ -2098,10 +2097,10 @@
         <v>67</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B42" s="23" t="s">
         <v>166</v>
       </c>
@@ -2112,10 +2111,10 @@
         <v>67</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" s="40" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" s="40" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B43" s="41" t="s">
         <v>167</v>
       </c>
@@ -2126,27 +2125,27 @@
         <v>67</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44" s="25"/>
       <c r="C44" s="20"/>
       <c r="D44" s="19"/>
       <c r="E44" s="20"/>
     </row>
-    <row r="45" spans="2:5" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B45" s="26"/>
       <c r="C45" s="21"/>
       <c r="E45" s="13"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="25"/>
       <c r="C46" s="20"/>
       <c r="D46" s="19"/>
       <c r="E46" s="20"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="25"/>
       <c r="C47" s="20"/>
       <c r="D47" s="19"/>
@@ -2162,7 +2161,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2172,14 +2171,14 @@
       <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.42578125" customWidth="1"/>
-    <col min="3" max="3" width="53.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.44140625" customWidth="1"/>
+    <col min="3" max="3" width="53.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>68</v>
       </c>
@@ -2193,7 +2192,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -2204,7 +2203,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -2215,7 +2214,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -2223,7 +2222,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -2231,7 +2230,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>59</v>
       </c>
@@ -2242,7 +2241,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>80</v>
       </c>
@@ -2250,7 +2249,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>82</v>
       </c>
@@ -2264,7 +2263,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>82</v>
       </c>
@@ -2278,7 +2277,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>82</v>
       </c>
@@ -2292,7 +2291,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>82</v>
       </c>
@@ -2306,7 +2305,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>82</v>
       </c>
@@ -2320,7 +2319,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>82</v>
       </c>
@@ -2334,7 +2333,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>82</v>
       </c>
@@ -2348,7 +2347,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>82</v>
       </c>
@@ -2362,7 +2361,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>82</v>
       </c>
@@ -2376,7 +2375,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>82</v>
       </c>
@@ -2390,7 +2389,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>82</v>
       </c>
@@ -2404,7 +2403,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
         <v>82</v>
       </c>
@@ -2418,7 +2417,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>63</v>
       </c>
@@ -2432,7 +2431,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
@@ -2446,7 +2445,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>63</v>
       </c>
@@ -2460,7 +2459,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>63</v>
       </c>
@@ -2474,7 +2473,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
@@ -2488,7 +2487,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>63</v>
       </c>
@@ -2502,7 +2501,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
@@ -2516,7 +2515,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>104</v>
       </c>
@@ -2527,7 +2526,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>104</v>
       </c>
@@ -2538,7 +2537,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>104</v>
       </c>
@@ -2549,7 +2548,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>104</v>
       </c>
@@ -2560,7 +2559,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>104</v>
       </c>
@@ -2571,7 +2570,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>104</v>
       </c>
@@ -2582,7 +2581,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>104</v>
       </c>
@@ -2593,7 +2592,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>104</v>
       </c>
@@ -2604,7 +2603,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>104</v>
       </c>
@@ -2615,7 +2614,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>104</v>
       </c>
@@ -2626,7 +2625,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>104</v>
       </c>
@@ -2637,7 +2636,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>104</v>
       </c>
@@ -2648,7 +2647,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>104</v>
       </c>
@@ -2659,7 +2658,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>104</v>
       </c>
@@ -2670,7 +2669,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>104</v>
       </c>
@@ -2681,7 +2680,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>104</v>
       </c>
@@ -2692,7 +2691,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>104</v>
       </c>
@@ -2703,7 +2702,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>104</v>
       </c>
@@ -2714,7 +2713,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>104</v>
       </c>
@@ -2725,7 +2724,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>104</v>
       </c>
@@ -2736,7 +2735,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>104</v>
       </c>
@@ -2747,7 +2746,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>104</v>
       </c>
@@ -2758,7 +2757,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>104</v>
       </c>
@@ -2769,7 +2768,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>104</v>
       </c>
@@ -2780,7 +2779,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>104</v>
       </c>
@@ -2791,7 +2790,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>104</v>
       </c>
@@ -2802,7 +2801,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>104</v>
       </c>
@@ -2813,7 +2812,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>104</v>
       </c>
@@ -2824,7 +2823,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>104</v>
       </c>
@@ -2835,7 +2834,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>104</v>
       </c>
@@ -2846,7 +2845,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>104</v>
       </c>
@@ -2857,7 +2856,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>104</v>
       </c>
@@ -2868,7 +2867,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>104</v>
       </c>
@@ -2879,7 +2878,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>104</v>
       </c>
@@ -2890,7 +2889,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>104</v>
       </c>
@@ -2901,7 +2900,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>104</v>
       </c>
@@ -2912,7 +2911,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>104</v>
       </c>
@@ -2923,7 +2922,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>104</v>
       </c>
@@ -2934,7 +2933,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>104</v>
       </c>
@@ -2945,7 +2944,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>104</v>
       </c>
@@ -2956,7 +2955,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>104</v>
       </c>
@@ -2967,7 +2966,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>104</v>
       </c>
@@ -2978,7 +2977,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>104</v>
       </c>
@@ -2989,7 +2988,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>104</v>
       </c>
@@ -3000,7 +2999,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>104</v>
       </c>
@@ -3011,7 +3010,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>104</v>
       </c>
@@ -3022,7 +3021,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>104</v>
       </c>
@@ -3033,7 +3032,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>104</v>
       </c>
@@ -3044,7 +3043,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>104</v>
       </c>
@@ -3055,7 +3054,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>104</v>
       </c>
@@ -3066,7 +3065,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>104</v>
       </c>
@@ -3077,7 +3076,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>104</v>
       </c>
@@ -3088,7 +3087,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>104</v>
       </c>
@@ -3099,7 +3098,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>104</v>
       </c>
@@ -3110,7 +3109,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>104</v>
       </c>
@@ -3121,7 +3120,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>161</v>
       </c>
@@ -3132,7 +3131,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="17" t="s">
         <v>161</v>
       </c>
@@ -3143,177 +3142,177 @@
         <v>163</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B85" t="s">
+        <v>220</v>
+      </c>
+      <c r="C85" t="s">
+        <v>219</v>
+      </c>
+      <c r="D85" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B86" t="s">
         <v>221</v>
       </c>
-      <c r="C85" t="s">
-        <v>220</v>
-      </c>
-      <c r="D85" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
+        <v>219</v>
+      </c>
+      <c r="D86" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B87" t="s">
         <v>222</v>
       </c>
-      <c r="C86" t="s">
-        <v>220</v>
-      </c>
-      <c r="D86" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
+        <v>219</v>
+      </c>
+      <c r="D87" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B88" t="s">
         <v>223</v>
       </c>
-      <c r="C87" t="s">
-        <v>220</v>
-      </c>
-      <c r="D87" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
+        <v>219</v>
+      </c>
+      <c r="D88" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B89" t="s">
         <v>224</v>
       </c>
-      <c r="C88" t="s">
-        <v>220</v>
-      </c>
-      <c r="D88" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
+        <v>219</v>
+      </c>
+      <c r="D89" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B90" t="s">
         <v>225</v>
       </c>
-      <c r="C89" t="s">
-        <v>220</v>
-      </c>
-      <c r="D89" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
+        <v>219</v>
+      </c>
+      <c r="D90" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B91" t="s">
         <v>226</v>
       </c>
-      <c r="C90" t="s">
-        <v>220</v>
-      </c>
-      <c r="D90" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
+        <v>219</v>
+      </c>
+      <c r="D91" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B92" t="s">
         <v>227</v>
       </c>
-      <c r="C91" t="s">
-        <v>220</v>
-      </c>
-      <c r="D91" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
+        <v>219</v>
+      </c>
+      <c r="D92" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B93" t="s">
         <v>228</v>
       </c>
-      <c r="C92" t="s">
-        <v>220</v>
-      </c>
-      <c r="D92" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B93" t="s">
+      <c r="C93" t="s">
+        <v>219</v>
+      </c>
+      <c r="D93" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B94" t="s">
         <v>229</v>
       </c>
-      <c r="C93" t="s">
-        <v>220</v>
-      </c>
-      <c r="D93" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
+        <v>219</v>
+      </c>
+      <c r="D94" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B95" t="s">
         <v>230</v>
       </c>
-      <c r="C94" t="s">
-        <v>220</v>
-      </c>
-      <c r="D94" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
+        <v>219</v>
+      </c>
+      <c r="D95" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B96" t="s">
         <v>231</v>
       </c>
-      <c r="C95" t="s">
-        <v>220</v>
-      </c>
-      <c r="D95" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B96" t="s">
+      <c r="C96" t="s">
+        <v>219</v>
+      </c>
+      <c r="D96" t="s">
         <v>232</v>
       </c>
-      <c r="C96" t="s">
-        <v>220</v>
-      </c>
-      <c r="D96" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D97" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -3323,15 +3322,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3586,27 +3582,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3631,9 +3621,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>